<commit_message>
Made ID changes for navigation
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="37">
   <si>
     <t>RunToTest</t>
   </si>
@@ -115,6 +115,27 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>UAT42092128</t>
+  </si>
+  <si>
+    <t>UAT42092129</t>
+  </si>
+  <si>
+    <t>UAT42092130</t>
+  </si>
+  <si>
+    <t>UAT42092131</t>
+  </si>
+  <si>
+    <t>UAT42092132</t>
+  </si>
+  <si>
+    <t>UAT42092133</t>
+  </si>
+  <si>
+    <t>UAT42092134</t>
   </si>
 </sst>
 </file>
@@ -432,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -559,7 +580,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
@@ -594,7 +615,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
@@ -694,6 +715,356 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>123</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>456</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>123</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>456</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <v>123</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13">
+        <v>456</v>
+      </c>
+      <c r="H13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14">
+        <v>123</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <v>456</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>123</v>
+      </c>
+      <c r="H16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <v>456</v>
+      </c>
+      <c r="H17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Handled spinner and Billet To
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="43">
   <si>
     <t>RunToTest</t>
   </si>
@@ -136,6 +136,24 @@
   </si>
   <si>
     <t>UAT42092134</t>
+  </si>
+  <si>
+    <t>UAT42092138</t>
+  </si>
+  <si>
+    <t>UAT42092140</t>
+  </si>
+  <si>
+    <t>UAT42092141</t>
+  </si>
+  <si>
+    <t>UAT42092142</t>
+  </si>
+  <si>
+    <t>UAT42092144</t>
+  </si>
+  <si>
+    <t>UAT42092143</t>
   </si>
 </sst>
 </file>
@@ -453,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1000,7 +1018,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -1035,7 +1053,7 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>28</v>
@@ -1065,6 +1083,216 @@
         <v>1</v>
       </c>
       <c r="K17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>123</v>
+      </c>
+      <c r="H18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19">
+        <v>456</v>
+      </c>
+      <c r="H19" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>123</v>
+      </c>
+      <c r="H20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21">
+        <v>456</v>
+      </c>
+      <c r="H21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22">
+        <v>123</v>
+      </c>
+      <c r="H22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23">
+        <v>456</v>
+      </c>
+      <c r="H23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Handled spinner and Billet To updated ID
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="48">
   <si>
     <t>RunToTest</t>
   </si>
@@ -154,6 +154,21 @@
   </si>
   <si>
     <t>UAT42092143</t>
+  </si>
+  <si>
+    <t>UAT42092145</t>
+  </si>
+  <si>
+    <t>UAT42092146</t>
+  </si>
+  <si>
+    <t>UAT42092147</t>
+  </si>
+  <si>
+    <t>UAT42092148</t>
+  </si>
+  <si>
+    <t>UAT42092149</t>
   </si>
 </sst>
 </file>
@@ -463,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1193,7 +1208,7 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
         <v>40</v>
@@ -1263,7 +1278,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
         <v>41</v>
@@ -1293,6 +1308,216 @@
         <v>1</v>
       </c>
       <c r="K23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24">
+        <v>123</v>
+      </c>
+      <c r="H24" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25">
+        <v>456</v>
+      </c>
+      <c r="H25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26">
+        <v>123</v>
+      </c>
+      <c r="H26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27">
+        <v>456</v>
+      </c>
+      <c r="H27" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28">
+        <v>123</v>
+      </c>
+      <c r="H28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29">
+        <v>456</v>
+      </c>
+      <c r="H29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" t="s">
+        <v>21</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Resolved chrome headless resolution
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="49">
   <si>
     <t>RunToTest</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>UAT42092149</t>
+  </si>
+  <si>
+    <t>UAT42092150</t>
   </si>
 </sst>
 </file>
@@ -478,7 +481,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -488,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1243,7 +1246,7 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
         <v>42</v>
@@ -1278,7 +1281,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>41</v>
@@ -1313,10 +1316,10 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -1348,10 +1351,10 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1386,7 +1389,7 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -1421,7 +1424,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -1456,7 +1459,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -1491,7 +1494,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Updated script based on logistic type
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -25,153 +25,288 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="94">
   <si>
     <t>RunToTest</t>
   </si>
   <si>
+    <t>BilledTo</t>
+  </si>
+  <si>
+    <t>ConsignmentID</t>
+  </si>
+  <si>
+    <t>CELW01</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>SenderName</t>
+  </si>
+  <si>
+    <t>ReceiverName</t>
+  </si>
+  <si>
+    <t>Surekha</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>ReceiverName2</t>
+  </si>
+  <si>
+    <t>Anand</t>
+  </si>
+  <si>
+    <t>UAT42092125</t>
+  </si>
+  <si>
+    <t>UAT42092135</t>
+  </si>
+  <si>
+    <t>ValueForCarrige</t>
+  </si>
+  <si>
+    <t>InvalidShipperReference</t>
+  </si>
+  <si>
+    <t>aaaaaa</t>
+  </si>
+  <si>
+    <t>wwww</t>
+  </si>
+  <si>
+    <t>ValidShipperReference</t>
+  </si>
+  <si>
+    <t>qqqqqqq</t>
+  </si>
+  <si>
+    <t>eeeeeee</t>
+  </si>
+  <si>
+    <t>NumberOfParcel</t>
+  </si>
+  <si>
+    <t>SecurityPack</t>
+  </si>
+  <si>
+    <t>SP12345678</t>
+  </si>
+  <si>
+    <t>UAT42092126</t>
+  </si>
+  <si>
+    <t>UAT42092136</t>
+  </si>
+  <si>
+    <t>UAT42092127</t>
+  </si>
+  <si>
+    <t>UAT42092137</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>UAT42092128</t>
+  </si>
+  <si>
+    <t>UAT42092129</t>
+  </si>
+  <si>
+    <t>UAT42092130</t>
+  </si>
+  <si>
+    <t>UAT42092131</t>
+  </si>
+  <si>
+    <t>UAT42092132</t>
+  </si>
+  <si>
+    <t>UAT42092133</t>
+  </si>
+  <si>
+    <t>UAT42092134</t>
+  </si>
+  <si>
+    <t>UAT42092138</t>
+  </si>
+  <si>
+    <t>UAT42092140</t>
+  </si>
+  <si>
+    <t>UAT42092141</t>
+  </si>
+  <si>
+    <t>UAT42092142</t>
+  </si>
+  <si>
+    <t>UAT42092144</t>
+  </si>
+  <si>
+    <t>UAT42092143</t>
+  </si>
+  <si>
+    <t>UAT42092145</t>
+  </si>
+  <si>
+    <t>UAT42092146</t>
+  </si>
+  <si>
+    <t>UAT42092147</t>
+  </si>
+  <si>
+    <t>UAT42092148</t>
+  </si>
+  <si>
+    <t>UAT42092149</t>
+  </si>
+  <si>
+    <t>UAT42092150</t>
+  </si>
+  <si>
+    <t>AIBT01</t>
+  </si>
+  <si>
+    <t>Sure</t>
+  </si>
+  <si>
+    <t>UAT42092151</t>
+  </si>
+  <si>
+    <t>UAT42092152</t>
+  </si>
+  <si>
+    <t>UAT42092153</t>
+  </si>
+  <si>
+    <t>UAT42092154</t>
+  </si>
+  <si>
+    <t>UAT42092155</t>
+  </si>
+  <si>
+    <t>UAT42092156</t>
+  </si>
+  <si>
+    <t>UAT42092157</t>
+  </si>
+  <si>
+    <t>UAT42092158</t>
+  </si>
+  <si>
+    <t>UAT42092159</t>
+  </si>
+  <si>
+    <t>UAT42092160</t>
+  </si>
+  <si>
+    <t>UAT42092161</t>
+  </si>
+  <si>
+    <t>UAT42092162</t>
+  </si>
+  <si>
+    <t>UAT42092163</t>
+  </si>
+  <si>
+    <t>UAT42092164</t>
+  </si>
+  <si>
+    <t>UAT42092165</t>
+  </si>
+  <si>
+    <t>UAT42092166</t>
+  </si>
+  <si>
+    <t>UAT42092167</t>
+  </si>
+  <si>
+    <t>UAT42092168</t>
+  </si>
+  <si>
+    <t>UAT42092169</t>
+  </si>
+  <si>
+    <t>UAT42092170</t>
+  </si>
+  <si>
+    <t>UAT42092171</t>
+  </si>
+  <si>
+    <t>UAT42092172</t>
+  </si>
+  <si>
+    <t>UAT42092173</t>
+  </si>
+  <si>
+    <t>UAT42092174</t>
+  </si>
+  <si>
+    <t>UAT42092175</t>
+  </si>
+  <si>
+    <t>UAT42092176</t>
+  </si>
+  <si>
+    <t>UAT42092177</t>
+  </si>
+  <si>
+    <t>UAT42092178</t>
+  </si>
+  <si>
+    <t>INTT02</t>
+  </si>
+  <si>
+    <t>UAT42092179</t>
+  </si>
+  <si>
+    <t>UAT42092180</t>
+  </si>
+  <si>
+    <t>UAT42092181</t>
+  </si>
+  <si>
+    <t>UAT42092182</t>
+  </si>
+  <si>
+    <t>UAT42092183</t>
+  </si>
+  <si>
+    <t>UAT42092184</t>
+  </si>
+  <si>
+    <t>UAT42092185</t>
+  </si>
+  <si>
+    <t>UAT42092186</t>
+  </si>
+  <si>
+    <t>UAT42092187</t>
+  </si>
+  <si>
+    <t>UAT42092189</t>
+  </si>
+  <si>
+    <t>UAT42092190</t>
+  </si>
+  <si>
+    <t>UAT42092191</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>BilledTo</t>
-  </si>
-  <si>
-    <t>ConsignmentID</t>
-  </si>
-  <si>
-    <t>CELW01</t>
-  </si>
-  <si>
-    <t>Cell</t>
-  </si>
-  <si>
-    <t>SenderName</t>
-  </si>
-  <si>
-    <t>ReceiverName</t>
-  </si>
-  <si>
-    <t>Surekha</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>ReceiverName2</t>
-  </si>
-  <si>
-    <t>Anand</t>
-  </si>
-  <si>
-    <t>UAT42092125</t>
-  </si>
-  <si>
-    <t>UAT42092135</t>
-  </si>
-  <si>
-    <t>ValueForCarrige</t>
-  </si>
-  <si>
-    <t>InvalidShipperReference</t>
-  </si>
-  <si>
-    <t>aaaaaa</t>
-  </si>
-  <si>
-    <t>wwww</t>
-  </si>
-  <si>
-    <t>ValidShipperReference</t>
-  </si>
-  <si>
-    <t>qqqqqqq</t>
-  </si>
-  <si>
-    <t>eeeeeee</t>
-  </si>
-  <si>
-    <t>NumberOfParcel</t>
-  </si>
-  <si>
-    <t>SecurityPack</t>
-  </si>
-  <si>
-    <t>SP12345678</t>
-  </si>
-  <si>
-    <t>UAT42092126</t>
-  </si>
-  <si>
-    <t>UAT42092136</t>
-  </si>
-  <si>
-    <t>UAT42092127</t>
-  </si>
-  <si>
-    <t>UAT42092137</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>UAT42092128</t>
-  </si>
-  <si>
-    <t>UAT42092129</t>
-  </si>
-  <si>
-    <t>UAT42092130</t>
-  </si>
-  <si>
-    <t>UAT42092131</t>
-  </si>
-  <si>
-    <t>UAT42092132</t>
-  </si>
-  <si>
-    <t>UAT42092133</t>
-  </si>
-  <si>
-    <t>UAT42092134</t>
-  </si>
-  <si>
-    <t>UAT42092138</t>
-  </si>
-  <si>
-    <t>UAT42092140</t>
-  </si>
-  <si>
-    <t>UAT42092141</t>
-  </si>
-  <si>
-    <t>UAT42092142</t>
-  </si>
-  <si>
-    <t>UAT42092144</t>
-  </si>
-  <si>
-    <t>UAT42092143</t>
-  </si>
-  <si>
-    <t>UAT42092145</t>
-  </si>
-  <si>
-    <t>UAT42092146</t>
-  </si>
-  <si>
-    <t>UAT42092147</t>
-  </si>
-  <si>
-    <t>UAT42092148</t>
-  </si>
-  <si>
-    <t>UAT42092149</t>
-  </si>
-  <si>
-    <t>UAT42092150</t>
+    <t>DIGI20</t>
+  </si>
+  <si>
+    <t>CELL</t>
   </si>
 </sst>
 </file>
@@ -489,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -514,1014 +649,2449 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
         <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2">
         <v>123</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3">
         <v>456</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4">
         <v>123</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5">
         <v>456</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6">
         <v>123</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7">
         <v>456</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
       <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8">
         <v>123</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9">
         <v>456</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
         <v>4</v>
       </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10">
         <v>123</v>
       </c>
       <c r="H10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11">
         <v>456</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G12">
         <v>123</v>
       </c>
       <c r="H12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G13">
         <v>456</v>
       </c>
       <c r="H13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
         <v>4</v>
       </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G14">
         <v>123</v>
       </c>
       <c r="H14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
         <v>4</v>
       </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G15">
         <v>456</v>
       </c>
       <c r="H15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G16">
         <v>123</v>
       </c>
       <c r="H16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J16">
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>456</v>
       </c>
       <c r="H17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J17">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
         <v>4</v>
       </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G18">
         <v>123</v>
       </c>
       <c r="H18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18">
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G19">
         <v>456</v>
       </c>
       <c r="H19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J19">
         <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
         <v>4</v>
       </c>
-      <c r="D20" t="s">
-        <v>5</v>
-      </c>
       <c r="E20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G20">
         <v>123</v>
       </c>
       <c r="H20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J20">
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
         <v>4</v>
       </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G21">
         <v>456</v>
       </c>
       <c r="H21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J21">
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
         <v>4</v>
       </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G22">
         <v>123</v>
       </c>
       <c r="H22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J22">
         <v>1</v>
       </c>
       <c r="K22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
         <v>4</v>
       </c>
-      <c r="D23" t="s">
-        <v>5</v>
-      </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G23">
         <v>456</v>
       </c>
       <c r="H23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J23">
         <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
         <v>4</v>
       </c>
-      <c r="D24" t="s">
-        <v>5</v>
-      </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G24">
         <v>123</v>
       </c>
       <c r="H24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J24">
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
-        <v>5</v>
-      </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G25">
         <v>456</v>
       </c>
       <c r="H25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J25">
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G26">
         <v>123</v>
       </c>
       <c r="H26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J26">
         <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G27">
         <v>456</v>
       </c>
       <c r="H27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J27">
         <v>1</v>
       </c>
       <c r="K27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G28">
         <v>123</v>
       </c>
       <c r="H28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J28">
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
         <v>48</v>
       </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G29">
         <v>456</v>
       </c>
       <c r="H29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J29">
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30">
+        <v>456</v>
+      </c>
+      <c r="H30" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31">
+        <v>456</v>
+      </c>
+      <c r="H31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32">
+        <v>456</v>
+      </c>
+      <c r="H32" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" t="s">
+        <v>20</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33">
+        <v>456</v>
+      </c>
+      <c r="H33" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34">
+        <v>456</v>
+      </c>
+      <c r="H34" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35">
+        <v>456</v>
+      </c>
+      <c r="H35" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36">
+        <v>456</v>
+      </c>
+      <c r="H36" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" t="s">
+        <v>20</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37">
+        <v>456</v>
+      </c>
+      <c r="H37" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" t="s">
+        <v>20</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38">
+        <v>456</v>
+      </c>
+      <c r="H38" t="s">
+        <v>17</v>
+      </c>
+      <c r="I38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39">
+        <v>456</v>
+      </c>
+      <c r="H39" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" t="s">
+        <v>20</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40">
+        <v>456</v>
+      </c>
+      <c r="H40" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41">
+        <v>456</v>
+      </c>
+      <c r="H41" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42">
+        <v>456</v>
+      </c>
+      <c r="H42" t="s">
+        <v>17</v>
+      </c>
+      <c r="I42" t="s">
+        <v>20</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43">
+        <v>456</v>
+      </c>
+      <c r="H43" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" t="s">
+        <v>20</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44">
+        <v>456</v>
+      </c>
+      <c r="H44" t="s">
+        <v>17</v>
+      </c>
+      <c r="I44" t="s">
+        <v>20</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45">
+        <v>456</v>
+      </c>
+      <c r="H45" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" t="s">
+        <v>20</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46">
+        <v>456</v>
+      </c>
+      <c r="H46" t="s">
+        <v>17</v>
+      </c>
+      <c r="I46" t="s">
+        <v>20</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47">
+        <v>456</v>
+      </c>
+      <c r="H47" t="s">
+        <v>17</v>
+      </c>
+      <c r="I47" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48">
+        <v>456</v>
+      </c>
+      <c r="H48" t="s">
+        <v>17</v>
+      </c>
+      <c r="I48" t="s">
+        <v>20</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A49" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49">
+        <v>456</v>
+      </c>
+      <c r="H49" t="s">
+        <v>17</v>
+      </c>
+      <c r="I49" t="s">
+        <v>20</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50">
+        <v>456</v>
+      </c>
+      <c r="H50" t="s">
+        <v>17</v>
+      </c>
+      <c r="I50" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A51" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51">
+        <v>456</v>
+      </c>
+      <c r="H51" t="s">
+        <v>17</v>
+      </c>
+      <c r="I51" t="s">
+        <v>20</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" t="s">
+        <v>28</v>
+      </c>
+      <c r="B52" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52">
+        <v>456</v>
+      </c>
+      <c r="H52" t="s">
+        <v>17</v>
+      </c>
+      <c r="I52" t="s">
+        <v>20</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A53" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53">
+        <v>456</v>
+      </c>
+      <c r="H53" t="s">
+        <v>17</v>
+      </c>
+      <c r="I53" t="s">
+        <v>20</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54">
+        <v>456</v>
+      </c>
+      <c r="H54" t="s">
+        <v>17</v>
+      </c>
+      <c r="I54" t="s">
+        <v>20</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s">
+        <v>49</v>
+      </c>
+      <c r="E55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55">
+        <v>456</v>
+      </c>
+      <c r="H55" t="s">
+        <v>17</v>
+      </c>
+      <c r="I55" t="s">
+        <v>20</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" t="s">
+        <v>49</v>
+      </c>
+      <c r="E56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56">
+        <v>456</v>
+      </c>
+      <c r="H56" t="s">
+        <v>17</v>
+      </c>
+      <c r="I56" t="s">
+        <v>20</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A57" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57">
+        <v>456</v>
+      </c>
+      <c r="H57" t="s">
+        <v>17</v>
+      </c>
+      <c r="I57" t="s">
+        <v>20</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A58" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" t="s">
+        <v>49</v>
+      </c>
+      <c r="E58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58">
+        <v>456</v>
+      </c>
+      <c r="H58" t="s">
+        <v>17</v>
+      </c>
+      <c r="I58" t="s">
+        <v>20</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A59" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" t="s">
+        <v>49</v>
+      </c>
+      <c r="E59" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59">
+        <v>456</v>
+      </c>
+      <c r="H59" t="s">
+        <v>17</v>
+      </c>
+      <c r="I59" t="s">
+        <v>20</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A60" t="s">
+        <v>28</v>
+      </c>
+      <c r="B60" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" t="s">
+        <v>49</v>
+      </c>
+      <c r="E60" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" t="s">
+        <v>93</v>
+      </c>
+      <c r="G60">
+        <v>456</v>
+      </c>
+      <c r="H60" t="s">
+        <v>17</v>
+      </c>
+      <c r="I60" t="s">
+        <v>20</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A61" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61">
+        <v>456</v>
+      </c>
+      <c r="H61" t="s">
+        <v>17</v>
+      </c>
+      <c r="I61" t="s">
+        <v>20</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A62" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" t="s">
+        <v>83</v>
+      </c>
+      <c r="C62" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62" t="s">
+        <v>49</v>
+      </c>
+      <c r="E62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" t="s">
+        <v>7</v>
+      </c>
+      <c r="G62">
+        <v>456</v>
+      </c>
+      <c r="H62" t="s">
+        <v>17</v>
+      </c>
+      <c r="I62" t="s">
+        <v>20</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="K62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A63" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" t="s">
+        <v>78</v>
+      </c>
+      <c r="D63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" t="s">
+        <v>7</v>
+      </c>
+      <c r="G63">
+        <v>456</v>
+      </c>
+      <c r="H63" t="s">
+        <v>17</v>
+      </c>
+      <c r="I63" t="s">
+        <v>20</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="K63" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64" t="s">
+        <v>49</v>
+      </c>
+      <c r="E64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64">
+        <v>456</v>
+      </c>
+      <c r="H64" t="s">
+        <v>17</v>
+      </c>
+      <c r="I64" t="s">
+        <v>20</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" t="s">
+        <v>78</v>
+      </c>
+      <c r="D65" t="s">
+        <v>49</v>
+      </c>
+      <c r="E65" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G65">
+        <v>456</v>
+      </c>
+      <c r="H65" t="s">
+        <v>17</v>
+      </c>
+      <c r="I65" t="s">
+        <v>20</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+      <c r="K65" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A66" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66" t="s">
+        <v>49</v>
+      </c>
+      <c r="E66" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66">
+        <v>456</v>
+      </c>
+      <c r="H66" t="s">
+        <v>17</v>
+      </c>
+      <c r="I66" t="s">
+        <v>20</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="K66" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A67" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" t="s">
+        <v>7</v>
+      </c>
+      <c r="G67">
+        <v>456</v>
+      </c>
+      <c r="H67" t="s">
+        <v>17</v>
+      </c>
+      <c r="I67" t="s">
+        <v>20</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+      <c r="K67" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A68" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" t="s">
+        <v>78</v>
+      </c>
+      <c r="D68" t="s">
+        <v>49</v>
+      </c>
+      <c r="E68" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" t="s">
+        <v>7</v>
+      </c>
+      <c r="G68">
+        <v>456</v>
+      </c>
+      <c r="H68" t="s">
+        <v>17</v>
+      </c>
+      <c r="I68" t="s">
+        <v>20</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+      <c r="K68" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A69" t="s">
+        <v>28</v>
+      </c>
+      <c r="B69" t="s">
+        <v>90</v>
+      </c>
+      <c r="C69" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" t="s">
+        <v>49</v>
+      </c>
+      <c r="E69" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" t="s">
+        <v>7</v>
+      </c>
+      <c r="G69">
+        <v>456</v>
+      </c>
+      <c r="H69" t="s">
+        <v>17</v>
+      </c>
+      <c r="I69" t="s">
+        <v>20</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A70" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" t="s">
+        <v>90</v>
+      </c>
+      <c r="C70" t="s">
+        <v>78</v>
+      </c>
+      <c r="D70" t="s">
+        <v>49</v>
+      </c>
+      <c r="E70" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" t="s">
+        <v>7</v>
+      </c>
+      <c r="G70">
+        <v>456</v>
+      </c>
+      <c r="H70" t="s">
+        <v>17</v>
+      </c>
+      <c r="I70" t="s">
+        <v>20</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Consignment Inbound script
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ConsignmentID" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="196">
   <si>
     <t>RunToTest</t>
   </si>
@@ -588,6 +588,33 @@
   </si>
   <si>
     <t>UAT42092199</t>
+  </si>
+  <si>
+    <t>UAT08000106</t>
+  </si>
+  <si>
+    <t>TestLast12</t>
+  </si>
+  <si>
+    <t>Nasreen11</t>
+  </si>
+  <si>
+    <t>UAT07000105</t>
+  </si>
+  <si>
+    <t>FNAutomation11</t>
+  </si>
+  <si>
+    <t>LNAutomation12</t>
+  </si>
+  <si>
+    <t>UAT42092202</t>
+  </si>
+  <si>
+    <t>UAT42092203</t>
+  </si>
+  <si>
+    <t>UAT42092204</t>
   </si>
 </sst>
 </file>
@@ -924,11 +951,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M78"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3685,7 +3712,7 @@
     </row>
     <row r="78" spans="1:13" ht="13.5" customHeight="1">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B78" t="s">
         <v>186</v>
@@ -3721,6 +3748,129 @@
         <v>1</v>
       </c>
       <c r="M78" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A79" t="s">
+        <v>28</v>
+      </c>
+      <c r="B79" t="s">
+        <v>193</v>
+      </c>
+      <c r="C79" t="s">
+        <v>94</v>
+      </c>
+      <c r="D79" t="s">
+        <v>173</v>
+      </c>
+      <c r="E79" t="s">
+        <v>170</v>
+      </c>
+      <c r="F79" t="s">
+        <v>95</v>
+      </c>
+      <c r="G79" t="s">
+        <v>9</v>
+      </c>
+      <c r="H79" t="s">
+        <v>96</v>
+      </c>
+      <c r="I79">
+        <v>456</v>
+      </c>
+      <c r="J79" t="s">
+        <v>17</v>
+      </c>
+      <c r="K79" t="s">
+        <v>20</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+      <c r="M79" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A80" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80" t="s">
+        <v>194</v>
+      </c>
+      <c r="C80" t="s">
+        <v>94</v>
+      </c>
+      <c r="D80" t="s">
+        <v>173</v>
+      </c>
+      <c r="E80" t="s">
+        <v>170</v>
+      </c>
+      <c r="F80" t="s">
+        <v>95</v>
+      </c>
+      <c r="G80" t="s">
+        <v>9</v>
+      </c>
+      <c r="H80" t="s">
+        <v>96</v>
+      </c>
+      <c r="I80">
+        <v>456</v>
+      </c>
+      <c r="J80" t="s">
+        <v>17</v>
+      </c>
+      <c r="K80" t="s">
+        <v>20</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="M80" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A81" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81" t="s">
+        <v>195</v>
+      </c>
+      <c r="C81" t="s">
+        <v>94</v>
+      </c>
+      <c r="D81" t="s">
+        <v>173</v>
+      </c>
+      <c r="E81" t="s">
+        <v>170</v>
+      </c>
+      <c r="F81" t="s">
+        <v>95</v>
+      </c>
+      <c r="G81" t="s">
+        <v>9</v>
+      </c>
+      <c r="H81" t="s">
+        <v>96</v>
+      </c>
+      <c r="I81">
+        <v>456</v>
+      </c>
+      <c r="J81" t="s">
+        <v>17</v>
+      </c>
+      <c r="K81" t="s">
+        <v>20</v>
+      </c>
+      <c r="L81">
+        <v>1</v>
+      </c>
+      <c r="M81" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3734,9 +3884,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="20100" topLeftCell="X1"/>
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H8" sqref="H8"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
@@ -4202,7 +4352,7 @@
     </row>
     <row r="7" spans="1:24" ht="45">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
         <v>183</v>
@@ -4274,27 +4424,78 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" ht="45">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>91</v>
+      </c>
+      <c r="B8" t="s">
+        <v>187</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" t="s">
+        <v>189</v>
+      </c>
+      <c r="I8" t="s">
+        <v>188</v>
+      </c>
+      <c r="J8" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L8" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N8" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O8" t="s">
+        <v>119</v>
+      </c>
+      <c r="P8" t="s">
+        <v>121</v>
       </c>
       <c r="Q8">
         <v>123</v>
       </c>
+      <c r="R8">
+        <v>987545555555555</v>
+      </c>
+      <c r="S8" t="s">
+        <v>124</v>
+      </c>
+      <c r="T8">
+        <v>1.11188888888888E+18</v>
+      </c>
       <c r="U8" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="V8" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="W8">
         <v>1</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -5842,9 +6043,11 @@
     <hyperlink ref="X6" r:id="rId10"/>
     <hyperlink ref="M7" r:id="rId11"/>
     <hyperlink ref="X7" r:id="rId12"/>
+    <hyperlink ref="M8" r:id="rId13"/>
+    <hyperlink ref="X8" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -5852,8 +6055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6167,7 +6370,7 @@
     </row>
     <row r="6" spans="1:19" ht="30">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>180</v>
@@ -6224,18 +6427,63 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" ht="30">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>91</v>
+      </c>
+      <c r="B7" t="s">
+        <v>190</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
-      </c>
-      <c r="N7" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I7" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K7" t="s">
+        <v>191</v>
+      </c>
+      <c r="L7" t="s">
+        <v>192</v>
+      </c>
+      <c r="M7">
+        <v>9876543210</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O7">
+        <v>107</v>
+      </c>
+      <c r="P7" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>129</v>
+      </c>
+      <c r="R7" t="s">
+        <v>148</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -7174,8 +7422,10 @@
     <hyperlink ref="N5" r:id="rId8"/>
     <hyperlink ref="J6" r:id="rId9"/>
     <hyperlink ref="N6" r:id="rId10"/>
+    <hyperlink ref="J7" r:id="rId11"/>
+    <hyperlink ref="N7" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Consignment Inbound script
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="223">
   <si>
     <t>RunToTest</t>
   </si>
@@ -654,6 +654,48 @@
   </si>
   <si>
     <t>UAT42092206</t>
+  </si>
+  <si>
+    <t>UAT42092207</t>
+  </si>
+  <si>
+    <t>UAT08000108</t>
+  </si>
+  <si>
+    <t>Nasreen15</t>
+  </si>
+  <si>
+    <t>TestLast16</t>
+  </si>
+  <si>
+    <t>UAT07000108</t>
+  </si>
+  <si>
+    <t>FNAutomation14</t>
+  </si>
+  <si>
+    <t>LNAutomation15</t>
+  </si>
+  <si>
+    <t>UAT07000109</t>
+  </si>
+  <si>
+    <t>FNAutomation15</t>
+  </si>
+  <si>
+    <t>LNAutomation16</t>
+  </si>
+  <si>
+    <t>UAT08000109</t>
+  </si>
+  <si>
+    <t>Nasreen16</t>
+  </si>
+  <si>
+    <t>TestLast17</t>
+  </si>
+  <si>
+    <t>UAT42092208</t>
   </si>
 </sst>
 </file>
@@ -982,7 +1024,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -990,11 +1032,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M83"/>
+  <dimension ref="A1:M85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
+      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3956,7 +3998,7 @@
     </row>
     <row r="83" spans="1:13" ht="13.5" customHeight="1">
       <c r="A83" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B83" t="s">
         <v>208</v>
@@ -3992,6 +4034,88 @@
         <v>1</v>
       </c>
       <c r="M83" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A84" t="s">
+        <v>28</v>
+      </c>
+      <c r="B84" t="s">
+        <v>209</v>
+      </c>
+      <c r="C84" t="s">
+        <v>94</v>
+      </c>
+      <c r="D84" t="s">
+        <v>173</v>
+      </c>
+      <c r="E84" t="s">
+        <v>170</v>
+      </c>
+      <c r="F84" t="s">
+        <v>95</v>
+      </c>
+      <c r="G84" t="s">
+        <v>9</v>
+      </c>
+      <c r="H84" t="s">
+        <v>96</v>
+      </c>
+      <c r="I84">
+        <v>456</v>
+      </c>
+      <c r="J84" t="s">
+        <v>17</v>
+      </c>
+      <c r="K84" t="s">
+        <v>20</v>
+      </c>
+      <c r="L84">
+        <v>1</v>
+      </c>
+      <c r="M84" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A85" t="s">
+        <v>91</v>
+      </c>
+      <c r="B85" t="s">
+        <v>222</v>
+      </c>
+      <c r="C85" t="s">
+        <v>94</v>
+      </c>
+      <c r="D85" t="s">
+        <v>173</v>
+      </c>
+      <c r="E85" t="s">
+        <v>170</v>
+      </c>
+      <c r="F85" t="s">
+        <v>95</v>
+      </c>
+      <c r="G85" t="s">
+        <v>9</v>
+      </c>
+      <c r="H85" t="s">
+        <v>96</v>
+      </c>
+      <c r="I85">
+        <v>456</v>
+      </c>
+      <c r="J85" t="s">
+        <v>17</v>
+      </c>
+      <c r="K85" t="s">
+        <v>20</v>
+      </c>
+      <c r="L85">
+        <v>1</v>
+      </c>
+      <c r="M85" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4007,7 +4131,7 @@
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <pane xSplit="20100" topLeftCell="X1"/>
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I12" sqref="I12"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
@@ -4695,7 +4819,7 @@
     </row>
     <row r="10" spans="1:24" ht="45">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>197</v>
@@ -4767,50 +4891,152 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" ht="45">
       <c r="A11" t="s">
         <v>28</v>
       </c>
+      <c r="B11" t="s">
+        <v>210</v>
+      </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11" t="s">
+        <v>211</v>
+      </c>
+      <c r="I11" t="s">
+        <v>212</v>
+      </c>
+      <c r="J11" t="s">
+        <v>111</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L11" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N11" t="s">
-        <v>11</v>
+        <v>96</v>
+      </c>
+      <c r="O11" t="s">
+        <v>119</v>
+      </c>
+      <c r="P11" t="s">
+        <v>121</v>
       </c>
       <c r="Q11">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R11">
+        <v>987545555555555</v>
+      </c>
+      <c r="S11" t="s">
+        <v>124</v>
+      </c>
+      <c r="T11">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U11" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V11" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="X11" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="45">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>91</v>
+      </c>
+      <c r="B12" t="s">
+        <v>219</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" t="s">
+        <v>220</v>
+      </c>
+      <c r="I12" t="s">
+        <v>221</v>
+      </c>
+      <c r="J12" t="s">
+        <v>111</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L12" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N12" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O12" t="s">
+        <v>119</v>
+      </c>
+      <c r="P12" t="s">
+        <v>121</v>
       </c>
       <c r="Q12">
         <v>123</v>
       </c>
+      <c r="R12">
+        <v>987545555555555</v>
+      </c>
+      <c r="S12" t="s">
+        <v>124</v>
+      </c>
+      <c r="T12">
+        <v>1.11188888888888E+18</v>
+      </c>
       <c r="U12" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="V12" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="W12">
         <v>1</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:24">
@@ -6272,9 +6498,13 @@
     <hyperlink ref="X9" r:id="rId16"/>
     <hyperlink ref="M10" r:id="rId17"/>
     <hyperlink ref="X10" r:id="rId18"/>
+    <hyperlink ref="M11" r:id="rId19"/>
+    <hyperlink ref="X11" r:id="rId20"/>
+    <hyperlink ref="M12" r:id="rId21"/>
+    <hyperlink ref="X12" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -6282,8 +6512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6774,7 +7004,7 @@
     </row>
     <row r="9" spans="1:19" ht="30">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>205</v>
@@ -6831,32 +7061,122 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" ht="30">
       <c r="A10" t="s">
         <v>28</v>
       </c>
+      <c r="B10" t="s">
+        <v>213</v>
+      </c>
       <c r="C10" t="s">
-        <v>94</v>
-      </c>
-      <c r="N10" s="1">
-        <v>123</v>
+        <v>125</v>
+      </c>
+      <c r="D10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G10" t="s">
+        <v>138</v>
+      </c>
+      <c r="H10" t="s">
+        <v>141</v>
+      </c>
+      <c r="I10" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K10" t="s">
+        <v>214</v>
+      </c>
+      <c r="L10" t="s">
+        <v>215</v>
+      </c>
+      <c r="M10">
+        <v>9876543210</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O10">
+        <v>107</v>
+      </c>
+      <c r="P10" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>129</v>
+      </c>
+      <c r="R10" t="s">
+        <v>148</v>
       </c>
       <c r="S10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="30">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
+        <v>216</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
-      </c>
-      <c r="N11" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" t="s">
+        <v>137</v>
+      </c>
+      <c r="G11" t="s">
+        <v>138</v>
+      </c>
+      <c r="H11" t="s">
+        <v>141</v>
+      </c>
+      <c r="I11" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K11" t="s">
+        <v>217</v>
+      </c>
+      <c r="L11" t="s">
+        <v>218</v>
+      </c>
+      <c r="M11">
+        <v>9876543210</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O11">
+        <v>107</v>
+      </c>
+      <c r="P11" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>129</v>
+      </c>
+      <c r="R11" t="s">
+        <v>148</v>
       </c>
       <c r="S11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -7745,8 +8065,12 @@
     <hyperlink ref="N8" r:id="rId14"/>
     <hyperlink ref="J9" r:id="rId15"/>
     <hyperlink ref="N9" r:id="rId16"/>
+    <hyperlink ref="J10" r:id="rId17"/>
+    <hyperlink ref="N10" r:id="rId18"/>
+    <hyperlink ref="J11" r:id="rId19"/>
+    <hyperlink ref="N11" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed loader timings in script
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ConsignmentID" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="315">
   <si>
     <t>RunToTest</t>
   </si>
@@ -696,6 +696,282 @@
   </si>
   <si>
     <t>UAT42092208</t>
+  </si>
+  <si>
+    <t>UAT42092209</t>
+  </si>
+  <si>
+    <t>UAT08000110</t>
+  </si>
+  <si>
+    <t>TestLast18</t>
+  </si>
+  <si>
+    <t>Nasreen17</t>
+  </si>
+  <si>
+    <t>FNAutomation16</t>
+  </si>
+  <si>
+    <t>LNAutomation17</t>
+  </si>
+  <si>
+    <t>UAT42092210</t>
+  </si>
+  <si>
+    <t>UAT42092211</t>
+  </si>
+  <si>
+    <t>UAT42092212</t>
+  </si>
+  <si>
+    <t>UAT42092213</t>
+  </si>
+  <si>
+    <t>UAT42092214</t>
+  </si>
+  <si>
+    <t>UAT42092215</t>
+  </si>
+  <si>
+    <t>UAT42092216</t>
+  </si>
+  <si>
+    <t>UAT42092217</t>
+  </si>
+  <si>
+    <t>UAT42092218</t>
+  </si>
+  <si>
+    <t>UAT42092219</t>
+  </si>
+  <si>
+    <t>UAT42092220</t>
+  </si>
+  <si>
+    <t>UAT08000111</t>
+  </si>
+  <si>
+    <t>UAT08000112</t>
+  </si>
+  <si>
+    <t>UAT08000113</t>
+  </si>
+  <si>
+    <t>UAT08000114</t>
+  </si>
+  <si>
+    <t>UAT08000115</t>
+  </si>
+  <si>
+    <t>UAT08000116</t>
+  </si>
+  <si>
+    <t>UAT08000117</t>
+  </si>
+  <si>
+    <t>UAT08000118</t>
+  </si>
+  <si>
+    <t>UAT08000119</t>
+  </si>
+  <si>
+    <t>UAT08000120</t>
+  </si>
+  <si>
+    <t>UAT08000121</t>
+  </si>
+  <si>
+    <t>UAT08000122</t>
+  </si>
+  <si>
+    <t>UAT08000123</t>
+  </si>
+  <si>
+    <t>TestLast19</t>
+  </si>
+  <si>
+    <t>TestLast20</t>
+  </si>
+  <si>
+    <t>TestLast21</t>
+  </si>
+  <si>
+    <t>TestLast22</t>
+  </si>
+  <si>
+    <t>TestLast23</t>
+  </si>
+  <si>
+    <t>TestLast24</t>
+  </si>
+  <si>
+    <t>TestLast25</t>
+  </si>
+  <si>
+    <t>TestLast26</t>
+  </si>
+  <si>
+    <t>TestLast27</t>
+  </si>
+  <si>
+    <t>TestLast28</t>
+  </si>
+  <si>
+    <t>TestLast29</t>
+  </si>
+  <si>
+    <t>TestLast30</t>
+  </si>
+  <si>
+    <t>TestLast31</t>
+  </si>
+  <si>
+    <t>Nasreen18</t>
+  </si>
+  <si>
+    <t>Nasreen19</t>
+  </si>
+  <si>
+    <t>Nasreen20</t>
+  </si>
+  <si>
+    <t>Nasreen21</t>
+  </si>
+  <si>
+    <t>Nasreen22</t>
+  </si>
+  <si>
+    <t>Nasreen23</t>
+  </si>
+  <si>
+    <t>Nasreen24</t>
+  </si>
+  <si>
+    <t>Nasreen25</t>
+  </si>
+  <si>
+    <t>Nasreen26</t>
+  </si>
+  <si>
+    <t>Nasreen27</t>
+  </si>
+  <si>
+    <t>Nasreen28</t>
+  </si>
+  <si>
+    <t>Nasreen29</t>
+  </si>
+  <si>
+    <t>Nasreen30</t>
+  </si>
+  <si>
+    <t>UAT07000110</t>
+  </si>
+  <si>
+    <t>UAT07000111</t>
+  </si>
+  <si>
+    <t>UAT07000112</t>
+  </si>
+  <si>
+    <t>UAT07000113</t>
+  </si>
+  <si>
+    <t>UAT07000114</t>
+  </si>
+  <si>
+    <t>UAT07000115</t>
+  </si>
+  <si>
+    <t>UAT07000116</t>
+  </si>
+  <si>
+    <t>UAT07000117</t>
+  </si>
+  <si>
+    <t>UAT07000118</t>
+  </si>
+  <si>
+    <t>UAT07000119</t>
+  </si>
+  <si>
+    <t>UAT07000120</t>
+  </si>
+  <si>
+    <t>UAT07000121</t>
+  </si>
+  <si>
+    <t>FNAutomation17</t>
+  </si>
+  <si>
+    <t>FNAutomation18</t>
+  </si>
+  <si>
+    <t>FNAutomation19</t>
+  </si>
+  <si>
+    <t>FNAutomation20</t>
+  </si>
+  <si>
+    <t>FNAutomation21</t>
+  </si>
+  <si>
+    <t>FNAutomation22</t>
+  </si>
+  <si>
+    <t>FNAutomation23</t>
+  </si>
+  <si>
+    <t>FNAutomation24</t>
+  </si>
+  <si>
+    <t>FNAutomation25</t>
+  </si>
+  <si>
+    <t>FNAutomation26</t>
+  </si>
+  <si>
+    <t>FNAutomation27</t>
+  </si>
+  <si>
+    <t>FNAutomation28</t>
+  </si>
+  <si>
+    <t>LNAutomation18</t>
+  </si>
+  <si>
+    <t>LNAutomation19</t>
+  </si>
+  <si>
+    <t>LNAutomation20</t>
+  </si>
+  <si>
+    <t>LNAutomation21</t>
+  </si>
+  <si>
+    <t>LNAutomation22</t>
+  </si>
+  <si>
+    <t>LNAutomation23</t>
+  </si>
+  <si>
+    <t>LNAutomation24</t>
+  </si>
+  <si>
+    <t>LNAutomation25</t>
+  </si>
+  <si>
+    <t>LNAutomation26</t>
+  </si>
+  <si>
+    <t>LNAutomation27</t>
+  </si>
+  <si>
+    <t>LNAutomation28</t>
+  </si>
+  <si>
+    <t>LNAutomation29</t>
   </si>
 </sst>
 </file>
@@ -1032,11 +1308,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4119,6 +4395,536 @@
         <v>23</v>
       </c>
     </row>
+    <row r="86" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A86" t="s">
+        <v>28</v>
+      </c>
+      <c r="B86" t="s">
+        <v>223</v>
+      </c>
+      <c r="C86" t="s">
+        <v>94</v>
+      </c>
+      <c r="D86" t="s">
+        <v>173</v>
+      </c>
+      <c r="E86" t="s">
+        <v>170</v>
+      </c>
+      <c r="F86" t="s">
+        <v>95</v>
+      </c>
+      <c r="G86" t="s">
+        <v>9</v>
+      </c>
+      <c r="H86" t="s">
+        <v>96</v>
+      </c>
+      <c r="I86">
+        <v>456</v>
+      </c>
+      <c r="J86" t="s">
+        <v>17</v>
+      </c>
+      <c r="K86" t="s">
+        <v>20</v>
+      </c>
+      <c r="L86">
+        <v>1</v>
+      </c>
+      <c r="M86" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A87" t="s">
+        <v>28</v>
+      </c>
+      <c r="B87" t="s">
+        <v>223</v>
+      </c>
+      <c r="C87" t="s">
+        <v>94</v>
+      </c>
+      <c r="D87" t="s">
+        <v>173</v>
+      </c>
+      <c r="E87" t="s">
+        <v>170</v>
+      </c>
+      <c r="F87" t="s">
+        <v>95</v>
+      </c>
+      <c r="G87" t="s">
+        <v>9</v>
+      </c>
+      <c r="H87" t="s">
+        <v>96</v>
+      </c>
+      <c r="I87">
+        <v>456</v>
+      </c>
+      <c r="J87" t="s">
+        <v>17</v>
+      </c>
+      <c r="K87" t="s">
+        <v>20</v>
+      </c>
+      <c r="L87">
+        <v>1</v>
+      </c>
+      <c r="M87" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A88" t="s">
+        <v>28</v>
+      </c>
+      <c r="B88" t="s">
+        <v>229</v>
+      </c>
+      <c r="C88" t="s">
+        <v>94</v>
+      </c>
+      <c r="D88" t="s">
+        <v>173</v>
+      </c>
+      <c r="E88" t="s">
+        <v>170</v>
+      </c>
+      <c r="F88" t="s">
+        <v>95</v>
+      </c>
+      <c r="G88" t="s">
+        <v>9</v>
+      </c>
+      <c r="H88" t="s">
+        <v>96</v>
+      </c>
+      <c r="I88">
+        <v>456</v>
+      </c>
+      <c r="J88" t="s">
+        <v>17</v>
+      </c>
+      <c r="K88" t="s">
+        <v>20</v>
+      </c>
+      <c r="L88">
+        <v>1</v>
+      </c>
+      <c r="M88" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A89" t="s">
+        <v>28</v>
+      </c>
+      <c r="B89" t="s">
+        <v>230</v>
+      </c>
+      <c r="C89" t="s">
+        <v>94</v>
+      </c>
+      <c r="D89" t="s">
+        <v>173</v>
+      </c>
+      <c r="E89" t="s">
+        <v>170</v>
+      </c>
+      <c r="F89" t="s">
+        <v>95</v>
+      </c>
+      <c r="G89" t="s">
+        <v>9</v>
+      </c>
+      <c r="H89" t="s">
+        <v>96</v>
+      </c>
+      <c r="I89">
+        <v>456</v>
+      </c>
+      <c r="J89" t="s">
+        <v>17</v>
+      </c>
+      <c r="K89" t="s">
+        <v>20</v>
+      </c>
+      <c r="L89">
+        <v>1</v>
+      </c>
+      <c r="M89" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A90" t="s">
+        <v>28</v>
+      </c>
+      <c r="B90" t="s">
+        <v>231</v>
+      </c>
+      <c r="C90" t="s">
+        <v>94</v>
+      </c>
+      <c r="D90" t="s">
+        <v>173</v>
+      </c>
+      <c r="E90" t="s">
+        <v>170</v>
+      </c>
+      <c r="F90" t="s">
+        <v>95</v>
+      </c>
+      <c r="G90" t="s">
+        <v>9</v>
+      </c>
+      <c r="H90" t="s">
+        <v>96</v>
+      </c>
+      <c r="I90">
+        <v>456</v>
+      </c>
+      <c r="J90" t="s">
+        <v>17</v>
+      </c>
+      <c r="K90" t="s">
+        <v>20</v>
+      </c>
+      <c r="L90">
+        <v>1</v>
+      </c>
+      <c r="M90" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A91" t="s">
+        <v>28</v>
+      </c>
+      <c r="B91" t="s">
+        <v>232</v>
+      </c>
+      <c r="C91" t="s">
+        <v>94</v>
+      </c>
+      <c r="D91" t="s">
+        <v>173</v>
+      </c>
+      <c r="E91" t="s">
+        <v>170</v>
+      </c>
+      <c r="F91" t="s">
+        <v>95</v>
+      </c>
+      <c r="G91" t="s">
+        <v>9</v>
+      </c>
+      <c r="H91" t="s">
+        <v>96</v>
+      </c>
+      <c r="I91">
+        <v>456</v>
+      </c>
+      <c r="J91" t="s">
+        <v>17</v>
+      </c>
+      <c r="K91" t="s">
+        <v>20</v>
+      </c>
+      <c r="L91">
+        <v>1</v>
+      </c>
+      <c r="M91" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A92" t="s">
+        <v>28</v>
+      </c>
+      <c r="B92" t="s">
+        <v>233</v>
+      </c>
+      <c r="C92" t="s">
+        <v>94</v>
+      </c>
+      <c r="D92" t="s">
+        <v>173</v>
+      </c>
+      <c r="E92" t="s">
+        <v>170</v>
+      </c>
+      <c r="F92" t="s">
+        <v>95</v>
+      </c>
+      <c r="G92" t="s">
+        <v>9</v>
+      </c>
+      <c r="H92" t="s">
+        <v>96</v>
+      </c>
+      <c r="I92">
+        <v>456</v>
+      </c>
+      <c r="J92" t="s">
+        <v>17</v>
+      </c>
+      <c r="K92" t="s">
+        <v>20</v>
+      </c>
+      <c r="L92">
+        <v>1</v>
+      </c>
+      <c r="M92" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A93" t="s">
+        <v>28</v>
+      </c>
+      <c r="B93" t="s">
+        <v>234</v>
+      </c>
+      <c r="C93" t="s">
+        <v>94</v>
+      </c>
+      <c r="D93" t="s">
+        <v>173</v>
+      </c>
+      <c r="E93" t="s">
+        <v>170</v>
+      </c>
+      <c r="F93" t="s">
+        <v>95</v>
+      </c>
+      <c r="G93" t="s">
+        <v>9</v>
+      </c>
+      <c r="H93" t="s">
+        <v>96</v>
+      </c>
+      <c r="I93">
+        <v>456</v>
+      </c>
+      <c r="J93" t="s">
+        <v>17</v>
+      </c>
+      <c r="K93" t="s">
+        <v>20</v>
+      </c>
+      <c r="L93">
+        <v>1</v>
+      </c>
+      <c r="M93" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A94" t="s">
+        <v>28</v>
+      </c>
+      <c r="B94" t="s">
+        <v>235</v>
+      </c>
+      <c r="C94" t="s">
+        <v>94</v>
+      </c>
+      <c r="D94" t="s">
+        <v>173</v>
+      </c>
+      <c r="E94" t="s">
+        <v>170</v>
+      </c>
+      <c r="F94" t="s">
+        <v>95</v>
+      </c>
+      <c r="G94" t="s">
+        <v>9</v>
+      </c>
+      <c r="H94" t="s">
+        <v>96</v>
+      </c>
+      <c r="I94">
+        <v>456</v>
+      </c>
+      <c r="J94" t="s">
+        <v>17</v>
+      </c>
+      <c r="K94" t="s">
+        <v>20</v>
+      </c>
+      <c r="L94">
+        <v>1</v>
+      </c>
+      <c r="M94" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="13.5" customHeight="1">
+      <c r="B95" t="s">
+        <v>236</v>
+      </c>
+      <c r="C95" t="s">
+        <v>94</v>
+      </c>
+      <c r="D95" t="s">
+        <v>173</v>
+      </c>
+      <c r="E95" t="s">
+        <v>170</v>
+      </c>
+      <c r="F95" t="s">
+        <v>95</v>
+      </c>
+      <c r="G95" t="s">
+        <v>9</v>
+      </c>
+      <c r="H95" t="s">
+        <v>96</v>
+      </c>
+      <c r="I95">
+        <v>456</v>
+      </c>
+      <c r="J95" t="s">
+        <v>17</v>
+      </c>
+      <c r="K95" t="s">
+        <v>20</v>
+      </c>
+      <c r="L95">
+        <v>1</v>
+      </c>
+      <c r="M95" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A96" t="s">
+        <v>28</v>
+      </c>
+      <c r="B96" t="s">
+        <v>237</v>
+      </c>
+      <c r="C96" t="s">
+        <v>94</v>
+      </c>
+      <c r="D96" t="s">
+        <v>173</v>
+      </c>
+      <c r="E96" t="s">
+        <v>170</v>
+      </c>
+      <c r="F96" t="s">
+        <v>95</v>
+      </c>
+      <c r="G96" t="s">
+        <v>9</v>
+      </c>
+      <c r="H96" t="s">
+        <v>96</v>
+      </c>
+      <c r="I96">
+        <v>456</v>
+      </c>
+      <c r="J96" t="s">
+        <v>17</v>
+      </c>
+      <c r="K96" t="s">
+        <v>20</v>
+      </c>
+      <c r="L96">
+        <v>1</v>
+      </c>
+      <c r="M96" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A97" t="s">
+        <v>28</v>
+      </c>
+      <c r="B97" t="s">
+        <v>238</v>
+      </c>
+      <c r="C97" t="s">
+        <v>94</v>
+      </c>
+      <c r="D97" t="s">
+        <v>173</v>
+      </c>
+      <c r="E97" t="s">
+        <v>170</v>
+      </c>
+      <c r="F97" t="s">
+        <v>95</v>
+      </c>
+      <c r="G97" t="s">
+        <v>9</v>
+      </c>
+      <c r="H97" t="s">
+        <v>96</v>
+      </c>
+      <c r="I97">
+        <v>456</v>
+      </c>
+      <c r="J97" t="s">
+        <v>17</v>
+      </c>
+      <c r="K97" t="s">
+        <v>20</v>
+      </c>
+      <c r="L97">
+        <v>1</v>
+      </c>
+      <c r="M97" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A98" t="s">
+        <v>28</v>
+      </c>
+      <c r="B98" t="s">
+        <v>239</v>
+      </c>
+      <c r="C98" t="s">
+        <v>94</v>
+      </c>
+      <c r="D98" t="s">
+        <v>173</v>
+      </c>
+      <c r="E98" t="s">
+        <v>170</v>
+      </c>
+      <c r="F98" t="s">
+        <v>95</v>
+      </c>
+      <c r="G98" t="s">
+        <v>9</v>
+      </c>
+      <c r="H98" t="s">
+        <v>96</v>
+      </c>
+      <c r="I98">
+        <v>456</v>
+      </c>
+      <c r="J98" t="s">
+        <v>17</v>
+      </c>
+      <c r="K98" t="s">
+        <v>20</v>
+      </c>
+      <c r="L98">
+        <v>1</v>
+      </c>
+      <c r="M98" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4129,9 +4935,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X73"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <pane xSplit="20100" topLeftCell="X1"/>
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A22" sqref="A22"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
@@ -5039,329 +5845,1040 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" ht="45">
       <c r="A13" t="s">
         <v>28</v>
       </c>
+      <c r="B13" t="s">
+        <v>224</v>
+      </c>
       <c r="C13" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" t="s">
+        <v>226</v>
+      </c>
+      <c r="I13" t="s">
+        <v>225</v>
+      </c>
+      <c r="J13" t="s">
+        <v>111</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L13" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N13" t="s">
-        <v>11</v>
+        <v>96</v>
+      </c>
+      <c r="O13" t="s">
+        <v>119</v>
+      </c>
+      <c r="P13" t="s">
+        <v>121</v>
       </c>
       <c r="Q13">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R13">
+        <v>987545555555555</v>
+      </c>
+      <c r="S13" t="s">
+        <v>124</v>
+      </c>
+      <c r="T13">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U13" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V13" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:24">
+      <c r="X13" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="45">
       <c r="A14" t="s">
         <v>28</v>
       </c>
+      <c r="B14" t="s">
+        <v>240</v>
+      </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" t="s">
+        <v>266</v>
+      </c>
+      <c r="I14" t="s">
+        <v>253</v>
+      </c>
+      <c r="J14" t="s">
+        <v>111</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L14" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N14" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O14" t="s">
+        <v>119</v>
+      </c>
+      <c r="P14" t="s">
+        <v>121</v>
       </c>
       <c r="Q14">
         <v>123</v>
       </c>
+      <c r="R14">
+        <v>987545555555555</v>
+      </c>
+      <c r="S14" t="s">
+        <v>124</v>
+      </c>
+      <c r="T14">
+        <v>1.11188888888888E+18</v>
+      </c>
       <c r="U14" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="V14" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="W14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:24">
+      <c r="X14" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="45">
       <c r="A15" t="s">
         <v>28</v>
       </c>
+      <c r="B15" t="s">
+        <v>241</v>
+      </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G15" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" t="s">
+        <v>267</v>
+      </c>
+      <c r="I15" t="s">
+        <v>254</v>
+      </c>
+      <c r="J15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L15" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N15" t="s">
-        <v>11</v>
+        <v>96</v>
+      </c>
+      <c r="O15" t="s">
+        <v>119</v>
+      </c>
+      <c r="P15" t="s">
+        <v>121</v>
       </c>
       <c r="Q15">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R15">
+        <v>987545555555555</v>
+      </c>
+      <c r="S15" t="s">
+        <v>124</v>
+      </c>
+      <c r="T15">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U15" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V15" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:24">
+      <c r="X15" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="45">
       <c r="A16" t="s">
         <v>28</v>
       </c>
+      <c r="B16" t="s">
+        <v>242</v>
+      </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" t="s">
+        <v>107</v>
+      </c>
+      <c r="H16" t="s">
+        <v>268</v>
+      </c>
+      <c r="I16" t="s">
+        <v>255</v>
+      </c>
+      <c r="J16" t="s">
+        <v>111</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L16" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N16" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O16" t="s">
+        <v>119</v>
+      </c>
+      <c r="P16" t="s">
+        <v>121</v>
       </c>
       <c r="Q16">
         <v>123</v>
       </c>
+      <c r="R16">
+        <v>987545555555555</v>
+      </c>
+      <c r="S16" t="s">
+        <v>124</v>
+      </c>
+      <c r="T16">
+        <v>1.11188888888888E+18</v>
+      </c>
       <c r="U16" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="V16" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="W16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:23">
+      <c r="X16" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="45">
       <c r="A17" t="s">
         <v>28</v>
       </c>
+      <c r="B17" t="s">
+        <v>243</v>
+      </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" t="s">
+        <v>269</v>
+      </c>
+      <c r="I17" t="s">
+        <v>256</v>
+      </c>
+      <c r="J17" t="s">
+        <v>111</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L17" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N17" t="s">
-        <v>11</v>
+        <v>96</v>
+      </c>
+      <c r="O17" t="s">
+        <v>119</v>
+      </c>
+      <c r="P17" t="s">
+        <v>121</v>
       </c>
       <c r="Q17">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R17">
+        <v>987545555555555</v>
+      </c>
+      <c r="S17" t="s">
+        <v>124</v>
+      </c>
+      <c r="T17">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U17" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V17" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:23">
+      <c r="X17" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="45">
       <c r="A18" t="s">
         <v>28</v>
       </c>
+      <c r="B18" t="s">
+        <v>244</v>
+      </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18" t="s">
+        <v>107</v>
+      </c>
+      <c r="H18" t="s">
+        <v>270</v>
+      </c>
+      <c r="I18" t="s">
+        <v>257</v>
+      </c>
+      <c r="J18" t="s">
+        <v>111</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L18" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N18" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O18" t="s">
+        <v>119</v>
+      </c>
+      <c r="P18" t="s">
+        <v>121</v>
       </c>
       <c r="Q18">
         <v>123</v>
       </c>
+      <c r="R18">
+        <v>987545555555555</v>
+      </c>
+      <c r="S18" t="s">
+        <v>124</v>
+      </c>
+      <c r="T18">
+        <v>1.11188888888888E+18</v>
+      </c>
       <c r="U18" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="V18" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="W18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:23">
+      <c r="X18" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="45">
       <c r="A19" t="s">
         <v>28</v>
       </c>
+      <c r="B19" t="s">
+        <v>245</v>
+      </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" t="s">
+        <v>271</v>
+      </c>
+      <c r="I19" t="s">
+        <v>258</v>
+      </c>
+      <c r="J19" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L19" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N19" t="s">
-        <v>11</v>
+        <v>96</v>
+      </c>
+      <c r="O19" t="s">
+        <v>119</v>
+      </c>
+      <c r="P19" t="s">
+        <v>121</v>
       </c>
       <c r="Q19">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R19">
+        <v>987545555555555</v>
+      </c>
+      <c r="S19" t="s">
+        <v>124</v>
+      </c>
+      <c r="T19">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U19" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V19" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:23">
+      <c r="X19" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="45">
       <c r="A20" t="s">
         <v>28</v>
       </c>
+      <c r="B20" t="s">
+        <v>246</v>
+      </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" t="s">
+        <v>107</v>
+      </c>
+      <c r="H20" t="s">
+        <v>272</v>
+      </c>
+      <c r="I20" t="s">
+        <v>259</v>
+      </c>
+      <c r="J20" t="s">
+        <v>111</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L20" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N20" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O20" t="s">
+        <v>119</v>
+      </c>
+      <c r="P20" t="s">
+        <v>121</v>
       </c>
       <c r="Q20">
         <v>123</v>
       </c>
+      <c r="R20">
+        <v>987545555555555</v>
+      </c>
+      <c r="S20" t="s">
+        <v>124</v>
+      </c>
+      <c r="T20">
+        <v>1.11188888888888E+18</v>
+      </c>
       <c r="U20" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="V20" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="W20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:23">
+      <c r="X20" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="45">
       <c r="A21" t="s">
         <v>28</v>
       </c>
+      <c r="B21" t="s">
+        <v>247</v>
+      </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" t="s">
+        <v>107</v>
+      </c>
+      <c r="H21" t="s">
+        <v>273</v>
+      </c>
+      <c r="I21" t="s">
+        <v>260</v>
+      </c>
+      <c r="J21" t="s">
+        <v>111</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L21" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N21" t="s">
-        <v>11</v>
+        <v>96</v>
+      </c>
+      <c r="O21" t="s">
+        <v>119</v>
+      </c>
+      <c r="P21" t="s">
+        <v>121</v>
       </c>
       <c r="Q21">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R21">
+        <v>987545555555555</v>
+      </c>
+      <c r="S21" t="s">
+        <v>124</v>
+      </c>
+      <c r="T21">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U21" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V21" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:23">
-      <c r="A22" t="s">
-        <v>28</v>
+      <c r="X21" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="45">
+      <c r="B22" t="s">
+        <v>248</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22" t="s">
+        <v>107</v>
+      </c>
+      <c r="H22" t="s">
+        <v>274</v>
+      </c>
+      <c r="I22" t="s">
+        <v>261</v>
+      </c>
+      <c r="J22" t="s">
+        <v>111</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L22" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N22" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O22" t="s">
+        <v>119</v>
+      </c>
+      <c r="P22" t="s">
+        <v>121</v>
       </c>
       <c r="Q22">
         <v>123</v>
       </c>
+      <c r="R22">
+        <v>987545555555555</v>
+      </c>
+      <c r="S22" t="s">
+        <v>124</v>
+      </c>
+      <c r="T22">
+        <v>1.11188888888888E+18</v>
+      </c>
       <c r="U22" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="V22" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="W22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:23">
+      <c r="X22" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="45">
       <c r="A23" t="s">
         <v>28</v>
       </c>
+      <c r="B23" t="s">
+        <v>249</v>
+      </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" t="s">
+        <v>126</v>
+      </c>
+      <c r="G23" t="s">
+        <v>107</v>
+      </c>
+      <c r="H23" t="s">
+        <v>275</v>
+      </c>
+      <c r="I23" t="s">
+        <v>262</v>
+      </c>
+      <c r="J23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L23" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N23" t="s">
-        <v>11</v>
+        <v>96</v>
+      </c>
+      <c r="O23" t="s">
+        <v>119</v>
+      </c>
+      <c r="P23" t="s">
+        <v>121</v>
       </c>
       <c r="Q23">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R23">
+        <v>987545555555555</v>
+      </c>
+      <c r="S23" t="s">
+        <v>124</v>
+      </c>
+      <c r="T23">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U23" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V23" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:23">
+      <c r="X23" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="45">
       <c r="A24" t="s">
         <v>28</v>
       </c>
+      <c r="B24" t="s">
+        <v>250</v>
+      </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" t="s">
+        <v>107</v>
+      </c>
+      <c r="H24" t="s">
+        <v>276</v>
+      </c>
+      <c r="I24" t="s">
+        <v>263</v>
+      </c>
+      <c r="J24" t="s">
+        <v>111</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L24" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N24" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O24" t="s">
+        <v>119</v>
+      </c>
+      <c r="P24" t="s">
+        <v>121</v>
       </c>
       <c r="Q24">
         <v>123</v>
       </c>
+      <c r="R24">
+        <v>987545555555555</v>
+      </c>
+      <c r="S24" t="s">
+        <v>124</v>
+      </c>
+      <c r="T24">
+        <v>1.11188888888888E+18</v>
+      </c>
       <c r="U24" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="V24" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="W24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:23">
+      <c r="X24" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" ht="45">
       <c r="A25" t="s">
         <v>28</v>
       </c>
+      <c r="B25" t="s">
+        <v>251</v>
+      </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" t="s">
+        <v>126</v>
+      </c>
+      <c r="G25" t="s">
+        <v>107</v>
+      </c>
+      <c r="H25" t="s">
+        <v>277</v>
+      </c>
+      <c r="I25" t="s">
+        <v>264</v>
+      </c>
+      <c r="J25" t="s">
+        <v>111</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L25" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N25" t="s">
-        <v>11</v>
+        <v>96</v>
+      </c>
+      <c r="O25" t="s">
+        <v>119</v>
+      </c>
+      <c r="P25" t="s">
+        <v>121</v>
       </c>
       <c r="Q25">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R25">
+        <v>987545555555555</v>
+      </c>
+      <c r="S25" t="s">
+        <v>124</v>
+      </c>
+      <c r="T25">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U25" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V25" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:23">
+      <c r="X25" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" ht="45">
       <c r="A26" t="s">
         <v>28</v>
       </c>
+      <c r="B26" t="s">
+        <v>252</v>
+      </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D26" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" t="s">
+        <v>126</v>
+      </c>
+      <c r="G26" t="s">
+        <v>107</v>
+      </c>
+      <c r="H26" t="s">
+        <v>278</v>
+      </c>
+      <c r="I26" t="s">
+        <v>265</v>
+      </c>
+      <c r="J26" t="s">
+        <v>111</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L26" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N26" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O26" t="s">
+        <v>119</v>
+      </c>
+      <c r="P26" t="s">
+        <v>121</v>
       </c>
       <c r="Q26">
         <v>123</v>
       </c>
+      <c r="R26">
+        <v>987545555555555</v>
+      </c>
+      <c r="S26" t="s">
+        <v>124</v>
+      </c>
+      <c r="T26">
+        <v>1.11188888888888E+18</v>
+      </c>
       <c r="U26" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="V26" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="W26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:23">
+      <c r="X26" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -5384,7 +6901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:24">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -5407,7 +6924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:24">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -5430,7 +6947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:24">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -5453,7 +6970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:24">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -5476,7 +6993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:24">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -6502,9 +8019,37 @@
     <hyperlink ref="X11" r:id="rId20"/>
     <hyperlink ref="M12" r:id="rId21"/>
     <hyperlink ref="X12" r:id="rId22"/>
+    <hyperlink ref="M13" r:id="rId23"/>
+    <hyperlink ref="X13" r:id="rId24"/>
+    <hyperlink ref="M14" r:id="rId25"/>
+    <hyperlink ref="M15" r:id="rId26"/>
+    <hyperlink ref="M16" r:id="rId27"/>
+    <hyperlink ref="M17" r:id="rId28"/>
+    <hyperlink ref="M18" r:id="rId29"/>
+    <hyperlink ref="M19" r:id="rId30"/>
+    <hyperlink ref="M20" r:id="rId31"/>
+    <hyperlink ref="M21" r:id="rId32"/>
+    <hyperlink ref="M22" r:id="rId33"/>
+    <hyperlink ref="M23" r:id="rId34"/>
+    <hyperlink ref="M24" r:id="rId35"/>
+    <hyperlink ref="M25" r:id="rId36"/>
+    <hyperlink ref="M26" r:id="rId37"/>
+    <hyperlink ref="X14" r:id="rId38"/>
+    <hyperlink ref="X15" r:id="rId39"/>
+    <hyperlink ref="X16" r:id="rId40"/>
+    <hyperlink ref="X17" r:id="rId41"/>
+    <hyperlink ref="X18" r:id="rId42"/>
+    <hyperlink ref="X19" r:id="rId43"/>
+    <hyperlink ref="X20" r:id="rId44"/>
+    <hyperlink ref="X21" r:id="rId45"/>
+    <hyperlink ref="X22" r:id="rId46"/>
+    <hyperlink ref="X23" r:id="rId47"/>
+    <hyperlink ref="X24" r:id="rId48"/>
+    <hyperlink ref="X25" r:id="rId49"/>
+    <hyperlink ref="X26" r:id="rId50"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId51"/>
 </worksheet>
 </file>
 
@@ -6512,8 +8057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7122,7 +8667,7 @@
     </row>
     <row r="11" spans="1:19" ht="30">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>216</v>
@@ -7179,186 +8724,768 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" ht="30">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>91</v>
+      </c>
+      <c r="B12" t="s">
+        <v>216</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
-      </c>
-      <c r="N12" s="1">
-        <v>123</v>
+        <v>125</v>
+      </c>
+      <c r="D12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G12" t="s">
+        <v>138</v>
+      </c>
+      <c r="H12" t="s">
+        <v>141</v>
+      </c>
+      <c r="I12" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K12" t="s">
+        <v>227</v>
+      </c>
+      <c r="L12" t="s">
+        <v>228</v>
+      </c>
+      <c r="M12">
+        <v>9876543210</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O12">
+        <v>107</v>
+      </c>
+      <c r="P12" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>129</v>
+      </c>
+      <c r="R12" t="s">
+        <v>148</v>
       </c>
       <c r="S12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="30">
       <c r="A13" t="s">
         <v>28</v>
       </c>
+      <c r="B13" t="s">
+        <v>279</v>
+      </c>
       <c r="C13" t="s">
-        <v>94</v>
-      </c>
-      <c r="N13" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" t="s">
+        <v>137</v>
+      </c>
+      <c r="G13" t="s">
+        <v>138</v>
+      </c>
+      <c r="H13" t="s">
+        <v>141</v>
+      </c>
+      <c r="I13" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K13" t="s">
+        <v>291</v>
+      </c>
+      <c r="L13" t="s">
+        <v>303</v>
+      </c>
+      <c r="M13">
+        <v>9876543210</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O13">
+        <v>107</v>
+      </c>
+      <c r="P13" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>129</v>
+      </c>
+      <c r="R13" t="s">
+        <v>148</v>
       </c>
       <c r="S13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="30">
       <c r="A14" t="s">
         <v>28</v>
       </c>
+      <c r="B14" t="s">
+        <v>280</v>
+      </c>
       <c r="C14" t="s">
-        <v>94</v>
-      </c>
-      <c r="N14" s="1">
-        <v>123</v>
+        <v>125</v>
+      </c>
+      <c r="D14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" t="s">
+        <v>138</v>
+      </c>
+      <c r="H14" t="s">
+        <v>141</v>
+      </c>
+      <c r="I14" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K14" t="s">
+        <v>292</v>
+      </c>
+      <c r="L14" t="s">
+        <v>304</v>
+      </c>
+      <c r="M14">
+        <v>9876543210</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O14">
+        <v>107</v>
+      </c>
+      <c r="P14" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>129</v>
+      </c>
+      <c r="R14" t="s">
+        <v>148</v>
       </c>
       <c r="S14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="30">
       <c r="A15" t="s">
         <v>28</v>
       </c>
+      <c r="B15" t="s">
+        <v>281</v>
+      </c>
       <c r="C15" t="s">
-        <v>94</v>
-      </c>
-      <c r="N15" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" t="s">
+        <v>138</v>
+      </c>
+      <c r="H15" t="s">
+        <v>141</v>
+      </c>
+      <c r="I15" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K15" t="s">
+        <v>293</v>
+      </c>
+      <c r="L15" t="s">
+        <v>305</v>
+      </c>
+      <c r="M15">
+        <v>9876543210</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O15">
+        <v>107</v>
+      </c>
+      <c r="P15" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>129</v>
+      </c>
+      <c r="R15" t="s">
+        <v>148</v>
       </c>
       <c r="S15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="30">
       <c r="A16" t="s">
         <v>28</v>
       </c>
+      <c r="B16" t="s">
+        <v>282</v>
+      </c>
       <c r="C16" t="s">
-        <v>94</v>
-      </c>
-      <c r="N16" s="1">
-        <v>123</v>
+        <v>125</v>
+      </c>
+      <c r="D16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G16" t="s">
+        <v>138</v>
+      </c>
+      <c r="H16" t="s">
+        <v>141</v>
+      </c>
+      <c r="I16" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K16" t="s">
+        <v>294</v>
+      </c>
+      <c r="L16" t="s">
+        <v>306</v>
+      </c>
+      <c r="M16">
+        <v>9876543210</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O16">
+        <v>107</v>
+      </c>
+      <c r="P16" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>129</v>
+      </c>
+      <c r="R16" t="s">
+        <v>148</v>
       </c>
       <c r="S16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="30">
       <c r="A17" t="s">
         <v>28</v>
       </c>
+      <c r="B17" t="s">
+        <v>283</v>
+      </c>
       <c r="C17" t="s">
-        <v>94</v>
-      </c>
-      <c r="N17" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" t="s">
+        <v>137</v>
+      </c>
+      <c r="G17" t="s">
+        <v>138</v>
+      </c>
+      <c r="H17" t="s">
+        <v>141</v>
+      </c>
+      <c r="I17" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K17" t="s">
+        <v>295</v>
+      </c>
+      <c r="L17" t="s">
+        <v>307</v>
+      </c>
+      <c r="M17">
+        <v>9876543210</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O17">
+        <v>107</v>
+      </c>
+      <c r="P17" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>129</v>
+      </c>
+      <c r="R17" t="s">
+        <v>148</v>
       </c>
       <c r="S17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="30">
       <c r="A18" t="s">
         <v>28</v>
       </c>
+      <c r="B18" t="s">
+        <v>284</v>
+      </c>
       <c r="C18" t="s">
-        <v>94</v>
-      </c>
-      <c r="N18" s="1">
-        <v>123</v>
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" t="s">
+        <v>137</v>
+      </c>
+      <c r="G18" t="s">
+        <v>138</v>
+      </c>
+      <c r="H18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I18" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K18" t="s">
+        <v>296</v>
+      </c>
+      <c r="L18" t="s">
+        <v>308</v>
+      </c>
+      <c r="M18">
+        <v>9876543210</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O18">
+        <v>107</v>
+      </c>
+      <c r="P18" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>129</v>
+      </c>
+      <c r="R18" t="s">
+        <v>148</v>
       </c>
       <c r="S18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="A19" t="s">
-        <v>28</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="30">
+      <c r="B19" t="s">
+        <v>285</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
-      </c>
-      <c r="N19" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" t="s">
+        <v>135</v>
+      </c>
+      <c r="F19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G19" t="s">
+        <v>138</v>
+      </c>
+      <c r="H19" t="s">
+        <v>141</v>
+      </c>
+      <c r="I19" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K19" t="s">
+        <v>297</v>
+      </c>
+      <c r="L19" t="s">
+        <v>309</v>
+      </c>
+      <c r="M19">
+        <v>9876543210</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O19">
+        <v>107</v>
+      </c>
+      <c r="P19" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>129</v>
+      </c>
+      <c r="R19" t="s">
+        <v>148</v>
       </c>
       <c r="S19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="30">
       <c r="A20" t="s">
         <v>28</v>
       </c>
+      <c r="B20" t="s">
+        <v>286</v>
+      </c>
       <c r="C20" t="s">
-        <v>94</v>
-      </c>
-      <c r="N20" s="1">
-        <v>123</v>
+        <v>125</v>
+      </c>
+      <c r="D20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" t="s">
+        <v>135</v>
+      </c>
+      <c r="F20" t="s">
+        <v>137</v>
+      </c>
+      <c r="G20" t="s">
+        <v>138</v>
+      </c>
+      <c r="H20" t="s">
+        <v>141</v>
+      </c>
+      <c r="I20" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K20" t="s">
+        <v>298</v>
+      </c>
+      <c r="L20" t="s">
+        <v>310</v>
+      </c>
+      <c r="M20">
+        <v>9876543210</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O20">
+        <v>107</v>
+      </c>
+      <c r="P20" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>129</v>
+      </c>
+      <c r="R20" t="s">
+        <v>148</v>
       </c>
       <c r="S20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="30">
       <c r="A21" t="s">
         <v>28</v>
       </c>
+      <c r="B21" t="s">
+        <v>287</v>
+      </c>
       <c r="C21" t="s">
-        <v>94</v>
-      </c>
-      <c r="N21" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" t="s">
+        <v>137</v>
+      </c>
+      <c r="G21" t="s">
+        <v>138</v>
+      </c>
+      <c r="H21" t="s">
+        <v>141</v>
+      </c>
+      <c r="I21" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K21" t="s">
+        <v>299</v>
+      </c>
+      <c r="L21" t="s">
+        <v>311</v>
+      </c>
+      <c r="M21">
+        <v>9876543210</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O21">
+        <v>107</v>
+      </c>
+      <c r="P21" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>129</v>
+      </c>
+      <c r="R21" t="s">
+        <v>148</v>
       </c>
       <c r="S21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="30">
       <c r="A22" t="s">
         <v>28</v>
       </c>
+      <c r="B22" t="s">
+        <v>288</v>
+      </c>
       <c r="C22" t="s">
-        <v>94</v>
-      </c>
-      <c r="N22" s="1">
-        <v>123</v>
+        <v>125</v>
+      </c>
+      <c r="D22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" t="s">
+        <v>137</v>
+      </c>
+      <c r="G22" t="s">
+        <v>138</v>
+      </c>
+      <c r="H22" t="s">
+        <v>141</v>
+      </c>
+      <c r="I22" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K22" t="s">
+        <v>300</v>
+      </c>
+      <c r="L22" t="s">
+        <v>312</v>
+      </c>
+      <c r="M22">
+        <v>9876543210</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O22">
+        <v>107</v>
+      </c>
+      <c r="P22" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>129</v>
+      </c>
+      <c r="R22" t="s">
+        <v>148</v>
       </c>
       <c r="S22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="30">
       <c r="A23" t="s">
         <v>28</v>
       </c>
+      <c r="B23" t="s">
+        <v>289</v>
+      </c>
       <c r="C23" t="s">
-        <v>94</v>
-      </c>
-      <c r="N23" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" t="s">
+        <v>137</v>
+      </c>
+      <c r="G23" t="s">
+        <v>138</v>
+      </c>
+      <c r="H23" t="s">
+        <v>141</v>
+      </c>
+      <c r="I23" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K23" t="s">
+        <v>301</v>
+      </c>
+      <c r="L23" t="s">
+        <v>313</v>
+      </c>
+      <c r="M23">
+        <v>9876543210</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O23">
+        <v>107</v>
+      </c>
+      <c r="P23" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>129</v>
+      </c>
+      <c r="R23" t="s">
+        <v>148</v>
       </c>
       <c r="S23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="30">
       <c r="A24" t="s">
         <v>28</v>
       </c>
+      <c r="B24" t="s">
+        <v>290</v>
+      </c>
       <c r="C24" t="s">
-        <v>94</v>
-      </c>
-      <c r="N24" s="1">
-        <v>123</v>
+        <v>125</v>
+      </c>
+      <c r="D24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24" t="s">
+        <v>137</v>
+      </c>
+      <c r="G24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H24" t="s">
+        <v>141</v>
+      </c>
+      <c r="I24" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K24" t="s">
+        <v>302</v>
+      </c>
+      <c r="L24" t="s">
+        <v>314</v>
+      </c>
+      <c r="M24">
+        <v>9876543210</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O24">
+        <v>107</v>
+      </c>
+      <c r="P24" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>129</v>
+      </c>
+      <c r="R24" t="s">
+        <v>148</v>
       </c>
       <c r="S24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -8069,8 +10196,34 @@
     <hyperlink ref="N10" r:id="rId18"/>
     <hyperlink ref="J11" r:id="rId19"/>
     <hyperlink ref="N11" r:id="rId20"/>
+    <hyperlink ref="J12" r:id="rId21"/>
+    <hyperlink ref="N12" r:id="rId22"/>
+    <hyperlink ref="J13" r:id="rId23"/>
+    <hyperlink ref="J14" r:id="rId24"/>
+    <hyperlink ref="J15" r:id="rId25"/>
+    <hyperlink ref="J16" r:id="rId26"/>
+    <hyperlink ref="J17" r:id="rId27"/>
+    <hyperlink ref="J18" r:id="rId28"/>
+    <hyperlink ref="J19" r:id="rId29"/>
+    <hyperlink ref="J20" r:id="rId30"/>
+    <hyperlink ref="J21" r:id="rId31"/>
+    <hyperlink ref="J22" r:id="rId32"/>
+    <hyperlink ref="J23" r:id="rId33"/>
+    <hyperlink ref="J24" r:id="rId34"/>
+    <hyperlink ref="N13" r:id="rId35"/>
+    <hyperlink ref="N14" r:id="rId36"/>
+    <hyperlink ref="N15" r:id="rId37"/>
+    <hyperlink ref="N16" r:id="rId38"/>
+    <hyperlink ref="N17" r:id="rId39"/>
+    <hyperlink ref="N18" r:id="rId40"/>
+    <hyperlink ref="N19" r:id="rId41"/>
+    <hyperlink ref="N20" r:id="rId42"/>
+    <hyperlink ref="N21" r:id="rId43"/>
+    <hyperlink ref="N22" r:id="rId44"/>
+    <hyperlink ref="N23" r:id="rId45"/>
+    <hyperlink ref="N24" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId47"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added commodity dorpdown scenerio
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="ConsignmentID" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2146" uniqueCount="315">
   <si>
     <t>RunToTest</t>
   </si>
@@ -1310,9 +1310,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4356,7 +4356,7 @@
     </row>
     <row r="85" spans="1:13" ht="13.5" customHeight="1">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B85" t="s">
         <v>222</v>
@@ -4765,6 +4765,9 @@
       </c>
     </row>
     <row r="95" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A95" t="s">
+        <v>28</v>
+      </c>
       <c r="B95" t="s">
         <v>236</v>
       </c>
@@ -4804,7 +4807,7 @@
     </row>
     <row r="96" spans="1:13" ht="13.5" customHeight="1">
       <c r="A96" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="B96" t="s">
         <v>237</v>
@@ -4935,7 +4938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X73"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <pane xSplit="20100" topLeftCell="X1"/>
       <selection activeCell="A22" sqref="A22"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
@@ -5773,7 +5776,7 @@
     </row>
     <row r="12" spans="1:24" ht="45">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>219</v>
@@ -6512,6 +6515,9 @@
       </c>
     </row>
     <row r="22" spans="1:24" ht="45">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
       <c r="B22" t="s">
         <v>248</v>
       </c>
@@ -8057,7 +8063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -8726,7 +8732,7 @@
     </row>
     <row r="12" spans="1:19" ht="30">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>216</v>
@@ -9138,6 +9144,9 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="30">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
       <c r="B19" t="s">
         <v>285</v>
       </c>

</xml_diff>

<commit_message>
Added commodity dropdown values
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19428" windowHeight="10428" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ConsignmentID" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="316">
   <si>
     <t>RunToTest</t>
   </si>
@@ -972,6 +972,9 @@
   </si>
   <si>
     <t>LNAutomation29</t>
+  </si>
+  <si>
+    <t>UAT42092221</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1303,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1308,26 +1311,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M98"/>
+  <dimension ref="A1:M99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.5546875" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.44140625" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -4356,7 +4359,7 @@
     </row>
     <row r="85" spans="1:13" ht="13.5" customHeight="1">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B85" t="s">
         <v>222</v>
@@ -4765,6 +4768,9 @@
       </c>
     </row>
     <row r="95" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A95" t="s">
+        <v>28</v>
+      </c>
       <c r="B95" t="s">
         <v>236</v>
       </c>
@@ -4922,6 +4928,47 @@
         <v>1</v>
       </c>
       <c r="M98" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A99" t="s">
+        <v>91</v>
+      </c>
+      <c r="B99" t="s">
+        <v>315</v>
+      </c>
+      <c r="C99" t="s">
+        <v>94</v>
+      </c>
+      <c r="D99" t="s">
+        <v>173</v>
+      </c>
+      <c r="E99" t="s">
+        <v>170</v>
+      </c>
+      <c r="F99" t="s">
+        <v>95</v>
+      </c>
+      <c r="G99" t="s">
+        <v>9</v>
+      </c>
+      <c r="H99" t="s">
+        <v>96</v>
+      </c>
+      <c r="I99">
+        <v>456</v>
+      </c>
+      <c r="J99" t="s">
+        <v>17</v>
+      </c>
+      <c r="K99" t="s">
+        <v>20</v>
+      </c>
+      <c r="L99">
+        <v>1</v>
+      </c>
+      <c r="M99" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4935,29 +4982,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X73"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <pane xSplit="20100" topLeftCell="X1"/>
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <pane xSplit="20112" topLeftCell="X1"/>
+      <selection activeCell="A24" sqref="A24"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
-    <col min="6" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="10" width="18.85546875" customWidth="1"/>
-    <col min="11" max="13" width="18.85546875" style="1" customWidth="1"/>
-    <col min="14" max="16" width="18.42578125" customWidth="1"/>
-    <col min="17" max="20" width="15.28515625" customWidth="1"/>
-    <col min="21" max="21" width="22.42578125" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" customWidth="1"/>
+    <col min="6" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="10" width="18.88671875" customWidth="1"/>
+    <col min="11" max="13" width="18.88671875" style="1" customWidth="1"/>
+    <col min="14" max="16" width="18.44140625" customWidth="1"/>
+    <col min="17" max="20" width="15.33203125" customWidth="1"/>
+    <col min="21" max="21" width="22.44140625" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" customWidth="1"/>
+    <col min="24" max="24" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="30">
+    <row r="1" spans="1:24" ht="28.8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5031,7 +5078,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="45">
+    <row r="2" spans="1:24" ht="43.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -5105,7 +5152,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="45">
+    <row r="3" spans="1:24" ht="43.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -5179,7 +5226,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="45">
+    <row r="4" spans="1:24" ht="43.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -5253,7 +5300,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="45">
+    <row r="5" spans="1:24" ht="43.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -5327,7 +5374,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="45">
+    <row r="6" spans="1:24" ht="43.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -5401,7 +5448,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="45">
+    <row r="7" spans="1:24" ht="43.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -5475,7 +5522,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="45">
+    <row r="8" spans="1:24" ht="43.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -5549,7 +5596,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="45">
+    <row r="9" spans="1:24" ht="43.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -5623,7 +5670,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="45">
+    <row r="10" spans="1:24" ht="43.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -5697,7 +5744,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="45">
+    <row r="11" spans="1:24" ht="43.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -5771,9 +5818,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="45">
+    <row r="12" spans="1:24" ht="43.2">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>219</v>
@@ -5845,7 +5892,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="45">
+    <row r="13" spans="1:24" ht="43.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -5919,7 +5966,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="45">
+    <row r="14" spans="1:24" ht="43.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -5993,7 +6040,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="45">
+    <row r="15" spans="1:24" ht="43.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -6067,7 +6114,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="45">
+    <row r="16" spans="1:24" ht="43.2">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -6141,7 +6188,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="45">
+    <row r="17" spans="1:24" ht="43.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -6215,7 +6262,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="45">
+    <row r="18" spans="1:24" ht="43.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -6289,7 +6336,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="45">
+    <row r="19" spans="1:24" ht="43.2">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -6363,7 +6410,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="45">
+    <row r="20" spans="1:24" ht="43.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -6437,7 +6484,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="45">
+    <row r="21" spans="1:24" ht="43.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -6511,7 +6558,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="45">
+    <row r="22" spans="1:24" ht="43.2">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
       <c r="B22" t="s">
         <v>248</v>
       </c>
@@ -6582,7 +6632,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="45">
+    <row r="23" spans="1:24" ht="43.2">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -6656,9 +6706,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="45">
+    <row r="24" spans="1:24" ht="43.2">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
         <v>250</v>
@@ -6730,7 +6780,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="45">
+    <row r="25" spans="1:24" ht="43.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -6804,7 +6854,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="45">
+    <row r="26" spans="1:24" ht="43.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -8057,25 +8107,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="8" width="18.85546875" customWidth="1"/>
-    <col min="9" max="10" width="18.85546875" style="1" customWidth="1"/>
-    <col min="11" max="13" width="18.42578125" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" style="1" customWidth="1"/>
-    <col min="15" max="18" width="15.28515625" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="8" width="18.88671875" customWidth="1"/>
+    <col min="9" max="10" width="18.88671875" style="1" customWidth="1"/>
+    <col min="11" max="13" width="18.44140625" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" style="1" customWidth="1"/>
+    <col min="15" max="18" width="15.33203125" customWidth="1"/>
+    <col min="19" max="19" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30">
+    <row r="1" spans="1:19" ht="28.8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8134,7 +8184,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="30">
+    <row r="2" spans="1:19" ht="28.8">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -8193,7 +8243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="30">
+    <row r="3" spans="1:19" ht="28.8">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -8252,7 +8302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="30">
+    <row r="4" spans="1:19" ht="28.8">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -8311,7 +8361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="30">
+    <row r="5" spans="1:19" ht="28.8">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -8370,7 +8420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="30">
+    <row r="6" spans="1:19" ht="28.8">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -8429,7 +8479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="30">
+    <row r="7" spans="1:19" ht="28.8">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -8488,7 +8538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="30">
+    <row r="8" spans="1:19" ht="28.8">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -8547,7 +8597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="30">
+    <row r="9" spans="1:19" ht="28.8">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -8606,7 +8656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="30">
+    <row r="10" spans="1:19" ht="28.8">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -8665,7 +8715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="30">
+    <row r="11" spans="1:19" ht="28.8">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -8724,9 +8774,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="30">
+    <row r="12" spans="1:19" ht="28.8">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>216</v>
@@ -8783,7 +8833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="30">
+    <row r="13" spans="1:19" ht="28.8">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -8842,7 +8892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="30">
+    <row r="14" spans="1:19" ht="28.8">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -8901,7 +8951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="30">
+    <row r="15" spans="1:19" ht="28.8">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -8960,7 +9010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="30">
+    <row r="16" spans="1:19" ht="28.8">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -9019,7 +9069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="30">
+    <row r="17" spans="1:19" ht="28.8">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -9078,7 +9128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="30">
+    <row r="18" spans="1:19" ht="28.8">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -9137,7 +9187,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="30">
+    <row r="19" spans="1:19" ht="28.8">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
       <c r="B19" t="s">
         <v>285</v>
       </c>
@@ -9193,9 +9246,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="30">
+    <row r="20" spans="1:19" ht="28.8">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
         <v>286</v>
@@ -9252,7 +9305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="30">
+    <row r="21" spans="1:19" ht="28.8">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -9311,7 +9364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="30">
+    <row r="22" spans="1:19" ht="28.8">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -9370,7 +9423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="30">
+    <row r="23" spans="1:19" ht="28.8">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -9429,7 +9482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="30">
+    <row r="24" spans="1:19" ht="28.8">
       <c r="A24" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added RMS test script updated consignmentID
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HardDiskCopied\E\InelliJ\SeleniumTestJavaArtifact2july\SeleniumTestJavaArtifact\DataFiles\excel\Login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F51FE1-8BD7-4F6C-AD58-DD33269BF796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977591B6-3966-4E05-8600-92E1FC50C7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="883" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3348" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3375" uniqueCount="460">
   <si>
     <t>RunToTest</t>
   </si>
@@ -1393,6 +1393,24 @@
   </si>
   <si>
     <t>LNAutomation39</t>
+  </si>
+  <si>
+    <t>UAT08000134</t>
+  </si>
+  <si>
+    <t>Nasreen42</t>
+  </si>
+  <si>
+    <t>TestLast43</t>
+  </si>
+  <si>
+    <t>UAT07000131</t>
+  </si>
+  <si>
+    <t>FNAutomation39</t>
+  </si>
+  <si>
+    <t>LNAutomation40</t>
   </si>
 </sst>
 </file>
@@ -1738,7 +1756,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1992,7 +2010,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
         <v>401</v>
@@ -2000,7 +2018,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
         <v>402</v>
@@ -2049,7 +2067,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
+      <selection pane="bottomLeft" activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6938,7 +6956,7 @@
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B130" t="s">
         <v>401</v>
@@ -6979,7 +6997,7 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="B131" t="s">
         <v>402</v>
@@ -9648,8 +9666,8 @@
   <dimension ref="A1:X73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12260,7 +12278,7 @@
     </row>
     <row r="36" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
         <v>448</v>
@@ -12332,27 +12350,78 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>454</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D37" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" t="s">
+        <v>126</v>
+      </c>
+      <c r="G37" t="s">
+        <v>107</v>
+      </c>
+      <c r="H37" t="s">
+        <v>455</v>
+      </c>
+      <c r="I37" t="s">
+        <v>456</v>
+      </c>
+      <c r="J37" t="s">
+        <v>111</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L37" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N37" t="s">
-        <v>11</v>
+        <v>96</v>
+      </c>
+      <c r="O37" t="s">
+        <v>119</v>
+      </c>
+      <c r="P37" t="s">
+        <v>121</v>
       </c>
       <c r="Q37">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R37">
+        <v>987545555555555</v>
+      </c>
+      <c r="S37" t="s">
+        <v>124</v>
+      </c>
+      <c r="T37">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U37" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V37" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W37">
         <v>1</v>
+      </c>
+      <c r="X37" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">
@@ -13291,9 +13360,11 @@
     <hyperlink ref="X35" r:id="rId68" xr:uid="{A238C700-6BD6-4A26-A081-CD84E25288ED}"/>
     <hyperlink ref="M36" r:id="rId69" xr:uid="{A9D4079E-1FDE-4B8C-A071-3482E1199727}"/>
     <hyperlink ref="X36" r:id="rId70" xr:uid="{B6B67919-C764-4E4C-AE7F-7B1D7B0D128D}"/>
+    <hyperlink ref="M37" r:id="rId71" xr:uid="{3536920E-9140-482A-88B2-59BC367F11B8}"/>
+    <hyperlink ref="X37" r:id="rId72" xr:uid="{73B7F698-FDA8-4524-B671-F285EF95F479}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId71"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId73"/>
 </worksheet>
 </file>
 
@@ -13301,8 +13372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15150,7 +15221,7 @@
     </row>
     <row r="32" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
         <v>451</v>
@@ -15207,18 +15278,63 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
+        <v>457</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
-      </c>
-      <c r="N33" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D33" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" t="s">
+        <v>135</v>
+      </c>
+      <c r="F33" t="s">
+        <v>137</v>
+      </c>
+      <c r="G33" t="s">
+        <v>138</v>
+      </c>
+      <c r="H33" t="s">
+        <v>141</v>
+      </c>
+      <c r="I33" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K33" t="s">
+        <v>458</v>
+      </c>
+      <c r="L33" t="s">
+        <v>459</v>
+      </c>
+      <c r="M33">
+        <v>9876543210</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O33">
+        <v>107</v>
+      </c>
+      <c r="P33" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>129</v>
+      </c>
+      <c r="R33" t="s">
+        <v>148</v>
       </c>
       <c r="S33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
@@ -15845,8 +15961,10 @@
     <hyperlink ref="N31" r:id="rId60" xr:uid="{25E4DD05-3367-42F2-8C02-2788221C129B}"/>
     <hyperlink ref="J32" r:id="rId61" xr:uid="{89B17850-2D69-480A-8B0F-E4AE8FD653F6}"/>
     <hyperlink ref="N32" r:id="rId62" xr:uid="{366C0470-F340-4D4F-A082-0308CCF3C69D}"/>
+    <hyperlink ref="J33" r:id="rId63" xr:uid="{1214DBD1-B565-4446-AA43-AFC07BB815F1}"/>
+    <hyperlink ref="N33" r:id="rId64" xr:uid="{7953C27C-5A89-45F5-A05C-0A1E62994517}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId63"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId65"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes RMS URL- test code
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HardDiskCopied\E\InelliJ\SeleniumTestJavaArtifact2july\SeleniumTestJavaArtifact\DataFiles\excel\Login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977591B6-3966-4E05-8600-92E1FC50C7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD409CE-26F8-4050-AA36-A46636564AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="883" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="883" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EditConsignmentUAT" sheetId="10" r:id="rId1"/>
@@ -2065,9 +2065,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A131" sqref="A131"/>
+      <selection pane="bottomLeft" activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13372,7 +13372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+    <sheetView topLeftCell="C25" workbookViewId="0">
       <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed RMS URL and updated consignmentID
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HardDiskCopied\E\InelliJ\SeleniumTestJavaArtifact2july\SeleniumTestJavaArtifact\DataFiles\excel\Login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD409CE-26F8-4050-AA36-A46636564AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87342966-FB76-4456-ACC5-A1F9B027B591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="883" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="883" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EditConsignmentUAT" sheetId="10" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3375" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3402" uniqueCount="466">
   <si>
     <t>RunToTest</t>
   </si>
@@ -1411,6 +1411,24 @@
   </si>
   <si>
     <t>LNAutomation40</t>
+  </si>
+  <si>
+    <t>UAT08000135</t>
+  </si>
+  <si>
+    <t>Nasreen43</t>
+  </si>
+  <si>
+    <t>TestLast44</t>
+  </si>
+  <si>
+    <t>UAT07000132</t>
+  </si>
+  <si>
+    <t>FNAutomation40</t>
+  </si>
+  <si>
+    <t>LNAutomation41</t>
   </si>
 </sst>
 </file>
@@ -1756,7 +1774,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2018,7 +2036,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
         <v>402</v>
@@ -2026,7 +2044,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
         <v>403</v>
@@ -2065,9 +2083,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B129" sqref="B129"/>
+      <selection pane="bottomLeft" activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6997,7 +7015,7 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B131" t="s">
         <v>402</v>
@@ -7038,7 +7056,7 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="B132" t="s">
         <v>403</v>
@@ -9667,7 +9685,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12352,7 +12370,7 @@
     </row>
     <row r="37" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
         <v>454</v>
@@ -12424,27 +12442,78 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
+        <v>460</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D38" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" t="s">
+        <v>126</v>
+      </c>
+      <c r="G38" t="s">
+        <v>107</v>
+      </c>
+      <c r="H38" t="s">
+        <v>461</v>
+      </c>
+      <c r="I38" t="s">
+        <v>462</v>
+      </c>
+      <c r="J38" t="s">
+        <v>111</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L38" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N38" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O38" t="s">
+        <v>119</v>
+      </c>
+      <c r="P38" t="s">
+        <v>121</v>
       </c>
       <c r="Q38">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R38">
+        <v>987545555555555</v>
+      </c>
+      <c r="S38" t="s">
+        <v>124</v>
+      </c>
+      <c r="T38">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U38" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V38" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W38">
         <v>1</v>
+      </c>
+      <c r="X38" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.3">
@@ -13362,9 +13431,11 @@
     <hyperlink ref="X36" r:id="rId70" xr:uid="{B6B67919-C764-4E4C-AE7F-7B1D7B0D128D}"/>
     <hyperlink ref="M37" r:id="rId71" xr:uid="{3536920E-9140-482A-88B2-59BC367F11B8}"/>
     <hyperlink ref="X37" r:id="rId72" xr:uid="{73B7F698-FDA8-4524-B671-F285EF95F479}"/>
+    <hyperlink ref="M38" r:id="rId73" xr:uid="{0E6DB531-58FE-4A44-9682-631C365C79B8}"/>
+    <hyperlink ref="X38" r:id="rId74" xr:uid="{DB8376BA-BCCC-4088-B32B-81E87DB9C814}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId73"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId75"/>
 </worksheet>
 </file>
 
@@ -13372,8 +13443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15280,7 +15351,7 @@
     </row>
     <row r="33" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
         <v>457</v>
@@ -15337,18 +15408,63 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>91</v>
+      </c>
+      <c r="B34" t="s">
+        <v>463</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
-      </c>
-      <c r="N34" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D34" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" t="s">
+        <v>135</v>
+      </c>
+      <c r="F34" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" t="s">
+        <v>138</v>
+      </c>
+      <c r="H34" t="s">
+        <v>141</v>
+      </c>
+      <c r="I34" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K34" t="s">
+        <v>464</v>
+      </c>
+      <c r="L34" t="s">
+        <v>465</v>
+      </c>
+      <c r="M34">
+        <v>9876543210</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O34">
+        <v>107</v>
+      </c>
+      <c r="P34" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>129</v>
+      </c>
+      <c r="R34" t="s">
+        <v>148</v>
       </c>
       <c r="S34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
@@ -15963,8 +16079,10 @@
     <hyperlink ref="N32" r:id="rId62" xr:uid="{366C0470-F340-4D4F-A082-0308CCF3C69D}"/>
     <hyperlink ref="J33" r:id="rId63" xr:uid="{1214DBD1-B565-4446-AA43-AFC07BB815F1}"/>
     <hyperlink ref="N33" r:id="rId64" xr:uid="{7953C27C-5A89-45F5-A05C-0A1E62994517}"/>
+    <hyperlink ref="J34" r:id="rId65" xr:uid="{1B9A4AFB-945B-48AF-A725-77D756323CD0}"/>
+    <hyperlink ref="N34" r:id="rId66" xr:uid="{01B859B6-7C7C-4D77-839E-7E48CED78722}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId65"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId67"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Prod changes- updated consignment
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HardDiskCopied\E\InelliJ\SeleniumTestJavaArtifact2july\SeleniumTestJavaArtifact\DataFiles\excel\Login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B1F454-2836-4069-95FB-199FE4A56A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D6991C-5C9E-44D6-A7F6-02750A86A756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="883" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="883" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EditConsignmentUAT" sheetId="10" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3567" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3594" uniqueCount="487">
   <si>
     <t>RunToTest</t>
   </si>
@@ -1476,9 +1476,6 @@
     <t>HQ11</t>
   </si>
   <si>
-    <t>HQ12</t>
-  </si>
-  <si>
     <t>PROD00011005</t>
   </si>
   <si>
@@ -1486,6 +1483,15 @@
   </si>
   <si>
     <t>PROD00021004</t>
+  </si>
+  <si>
+    <t>PROD00021005</t>
+  </si>
+  <si>
+    <t>PROD00011006</t>
+  </si>
+  <si>
+    <t>HQ13</t>
   </si>
 </sst>
 </file>
@@ -7285,8 +7291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE03A24-5145-4BFC-B798-CD5C2D481D00}">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7696,10 +7702,10 @@
     </row>
     <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>337</v>
@@ -7726,6 +7732,41 @@
         <v>338</v>
       </c>
       <c r="K12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="H13" s="1">
+        <v>400</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="K13" s="1">
         <v>3</v>
       </c>
     </row>
@@ -7793,7 +7834,7 @@
   <dimension ref="A1:X73"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8776,10 +8817,10 @@
     </row>
     <row r="14" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C14" t="s">
         <v>346</v>
@@ -8848,8 +8889,76 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="M15" s="2"/>
+    <row r="15" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" t="s">
+        <v>485</v>
+      </c>
+      <c r="C15" t="s">
+        <v>346</v>
+      </c>
+      <c r="D15" t="s">
+        <v>341</v>
+      </c>
+      <c r="E15" t="s">
+        <v>342</v>
+      </c>
+      <c r="F15" t="s">
+        <v>332</v>
+      </c>
+      <c r="G15" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" t="s">
+        <v>138</v>
+      </c>
+      <c r="I15" t="s">
+        <v>141</v>
+      </c>
+      <c r="J15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L15" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="N15" t="s">
+        <v>359</v>
+      </c>
+      <c r="O15" t="s">
+        <v>343</v>
+      </c>
+      <c r="P15" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q15">
+        <v>123</v>
+      </c>
+      <c r="R15">
+        <v>987545555555555</v>
+      </c>
+      <c r="S15" t="s">
+        <v>124</v>
+      </c>
+      <c r="T15">
+        <v>1.11188888888888E+18</v>
+      </c>
+      <c r="U15" t="s">
+        <v>128</v>
+      </c>
+      <c r="V15" t="s">
+        <v>129</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
       <c r="X15" s="3" t="s">
         <v>116</v>
       </c>
@@ -8961,44 +9070,45 @@
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" xr:uid="{358998FA-15FF-431B-99C1-DF0C84EFB86F}"/>
     <hyperlink ref="X2" r:id="rId2" xr:uid="{AE14EEEB-3B83-40AE-9BDF-EA985C28F832}"/>
-    <hyperlink ref="X15" r:id="rId3" xr:uid="{DAF1D1C9-089E-49E4-9D9E-E10F75BDD751}"/>
-    <hyperlink ref="X16" r:id="rId4" xr:uid="{19361FA6-9504-453F-92E7-DF6E9F4FA63D}"/>
-    <hyperlink ref="X17" r:id="rId5" xr:uid="{F402E61A-6BC9-41B2-87DF-C3A27E532E13}"/>
-    <hyperlink ref="X18" r:id="rId6" xr:uid="{43A3EAE1-5CC3-4836-A288-2BF5FC280717}"/>
-    <hyperlink ref="X19" r:id="rId7" xr:uid="{6F5EC072-9F18-4EC5-8DB2-2DF2CBF01CB0}"/>
-    <hyperlink ref="X20" r:id="rId8" xr:uid="{4CA5FEE5-0C07-4808-9248-B660743F3774}"/>
-    <hyperlink ref="X21" r:id="rId9" xr:uid="{ED490A4D-F92A-47BE-9867-4314A59BC6B7}"/>
-    <hyperlink ref="X22" r:id="rId10" xr:uid="{46880446-6A4E-403B-ADFA-CE8197023B30}"/>
-    <hyperlink ref="X23" r:id="rId11" xr:uid="{9524D2D4-0229-4303-A39E-B5869A5AB6F9}"/>
-    <hyperlink ref="X24" r:id="rId12" xr:uid="{918DE3BD-31B5-4450-94FD-FF0C378CE62A}"/>
-    <hyperlink ref="X25" r:id="rId13" xr:uid="{6DCC4064-F791-487D-8795-51EDAB204E8F}"/>
-    <hyperlink ref="X26" r:id="rId14" xr:uid="{CDB54460-A79F-4C90-B70B-EEBEE40D5E15}"/>
-    <hyperlink ref="X27" r:id="rId15" xr:uid="{020E49A6-F847-4012-A984-5906C66B24C2}"/>
-    <hyperlink ref="X28" r:id="rId16" xr:uid="{116CD7FA-45D6-45D0-9F78-90290FDE7EC3}"/>
-    <hyperlink ref="M3" r:id="rId17" xr:uid="{B6C5C0C4-A5CD-4989-9129-C8A7A85B04B8}"/>
-    <hyperlink ref="X3" r:id="rId18" xr:uid="{2F3B3A48-891E-47E7-8670-CEDB6572CA2B}"/>
-    <hyperlink ref="M4" r:id="rId19" xr:uid="{6A74C82A-96E6-471E-8814-621213BF313E}"/>
-    <hyperlink ref="X4" r:id="rId20" xr:uid="{FD29A6B0-0DCE-4017-BE5D-844FE8F434EA}"/>
-    <hyperlink ref="M5" r:id="rId21" xr:uid="{06767FBB-30D3-4571-B179-8F6EB3FEC4B4}"/>
-    <hyperlink ref="X5" r:id="rId22" xr:uid="{8840BE2F-FC00-482D-8632-9DB48E041BCA}"/>
-    <hyperlink ref="M6" r:id="rId23" xr:uid="{0A59FE27-88F7-4F24-A496-311F958815C8}"/>
-    <hyperlink ref="X6" r:id="rId24" xr:uid="{8DC3250D-4424-4A6C-B68D-FEC080B637FA}"/>
-    <hyperlink ref="M7" r:id="rId25" xr:uid="{4DC610F6-9A84-4368-BDF1-FF9BB2560852}"/>
-    <hyperlink ref="X7" r:id="rId26" xr:uid="{0FC8FA66-5837-4A59-BD4F-2E68649B972A}"/>
-    <hyperlink ref="M8" r:id="rId27" xr:uid="{88F825E6-41C8-4F6A-96AE-F0685382C2FB}"/>
-    <hyperlink ref="X8" r:id="rId28" xr:uid="{BF022674-73DC-417D-AA01-42951A83A5A9}"/>
-    <hyperlink ref="M9" r:id="rId29" xr:uid="{FA4C93BE-D55C-4CEF-901E-0EE7890E7319}"/>
-    <hyperlink ref="X9" r:id="rId30" xr:uid="{FE2E5242-2733-429A-B446-49922A127C38}"/>
-    <hyperlink ref="M10" r:id="rId31" xr:uid="{38AAA3EB-9E30-46B7-9C48-8E21BCE16101}"/>
-    <hyperlink ref="X10" r:id="rId32" xr:uid="{465D83FD-48FF-48EE-A4AA-EE7AF90F5BBD}"/>
-    <hyperlink ref="X11" r:id="rId33" xr:uid="{A8D2FF8B-A2A9-4B6F-B217-2E14C6EE9235}"/>
-    <hyperlink ref="M11" r:id="rId34" xr:uid="{175F9C8E-DB2C-48B2-B5D8-B249A4302B95}"/>
-    <hyperlink ref="X12" r:id="rId35" xr:uid="{E8D52455-2D02-474B-887B-F66CB5AB7BF3}"/>
-    <hyperlink ref="M12" r:id="rId36" xr:uid="{E9C6333C-597D-41EE-B1FC-1EE6178B208F}"/>
-    <hyperlink ref="X13" r:id="rId37" xr:uid="{8F2202D7-9DB8-441F-A802-398ADF2EFB9B}"/>
-    <hyperlink ref="M13" r:id="rId38" xr:uid="{5D30A358-A0BD-4F64-98E8-9F16E791B106}"/>
-    <hyperlink ref="X14" r:id="rId39" xr:uid="{104DBC51-97D1-4A7F-9676-DA2144C8BCF2}"/>
-    <hyperlink ref="M14" r:id="rId40" xr:uid="{D24A006E-62D8-4CFC-ADF2-379D45B10FF0}"/>
+    <hyperlink ref="X16" r:id="rId3" xr:uid="{19361FA6-9504-453F-92E7-DF6E9F4FA63D}"/>
+    <hyperlink ref="X17" r:id="rId4" xr:uid="{F402E61A-6BC9-41B2-87DF-C3A27E532E13}"/>
+    <hyperlink ref="X18" r:id="rId5" xr:uid="{43A3EAE1-5CC3-4836-A288-2BF5FC280717}"/>
+    <hyperlink ref="X19" r:id="rId6" xr:uid="{6F5EC072-9F18-4EC5-8DB2-2DF2CBF01CB0}"/>
+    <hyperlink ref="X20" r:id="rId7" xr:uid="{4CA5FEE5-0C07-4808-9248-B660743F3774}"/>
+    <hyperlink ref="X21" r:id="rId8" xr:uid="{ED490A4D-F92A-47BE-9867-4314A59BC6B7}"/>
+    <hyperlink ref="X22" r:id="rId9" xr:uid="{46880446-6A4E-403B-ADFA-CE8197023B30}"/>
+    <hyperlink ref="X23" r:id="rId10" xr:uid="{9524D2D4-0229-4303-A39E-B5869A5AB6F9}"/>
+    <hyperlink ref="X24" r:id="rId11" xr:uid="{918DE3BD-31B5-4450-94FD-FF0C378CE62A}"/>
+    <hyperlink ref="X25" r:id="rId12" xr:uid="{6DCC4064-F791-487D-8795-51EDAB204E8F}"/>
+    <hyperlink ref="X26" r:id="rId13" xr:uid="{CDB54460-A79F-4C90-B70B-EEBEE40D5E15}"/>
+    <hyperlink ref="X27" r:id="rId14" xr:uid="{020E49A6-F847-4012-A984-5906C66B24C2}"/>
+    <hyperlink ref="X28" r:id="rId15" xr:uid="{116CD7FA-45D6-45D0-9F78-90290FDE7EC3}"/>
+    <hyperlink ref="M3" r:id="rId16" xr:uid="{B6C5C0C4-A5CD-4989-9129-C8A7A85B04B8}"/>
+    <hyperlink ref="X3" r:id="rId17" xr:uid="{2F3B3A48-891E-47E7-8670-CEDB6572CA2B}"/>
+    <hyperlink ref="M4" r:id="rId18" xr:uid="{6A74C82A-96E6-471E-8814-621213BF313E}"/>
+    <hyperlink ref="X4" r:id="rId19" xr:uid="{FD29A6B0-0DCE-4017-BE5D-844FE8F434EA}"/>
+    <hyperlink ref="M5" r:id="rId20" xr:uid="{06767FBB-30D3-4571-B179-8F6EB3FEC4B4}"/>
+    <hyperlink ref="X5" r:id="rId21" xr:uid="{8840BE2F-FC00-482D-8632-9DB48E041BCA}"/>
+    <hyperlink ref="M6" r:id="rId22" xr:uid="{0A59FE27-88F7-4F24-A496-311F958815C8}"/>
+    <hyperlink ref="X6" r:id="rId23" xr:uid="{8DC3250D-4424-4A6C-B68D-FEC080B637FA}"/>
+    <hyperlink ref="M7" r:id="rId24" xr:uid="{4DC610F6-9A84-4368-BDF1-FF9BB2560852}"/>
+    <hyperlink ref="X7" r:id="rId25" xr:uid="{0FC8FA66-5837-4A59-BD4F-2E68649B972A}"/>
+    <hyperlink ref="M8" r:id="rId26" xr:uid="{88F825E6-41C8-4F6A-96AE-F0685382C2FB}"/>
+    <hyperlink ref="X8" r:id="rId27" xr:uid="{BF022674-73DC-417D-AA01-42951A83A5A9}"/>
+    <hyperlink ref="M9" r:id="rId28" xr:uid="{FA4C93BE-D55C-4CEF-901E-0EE7890E7319}"/>
+    <hyperlink ref="X9" r:id="rId29" xr:uid="{FE2E5242-2733-429A-B446-49922A127C38}"/>
+    <hyperlink ref="M10" r:id="rId30" xr:uid="{38AAA3EB-9E30-46B7-9C48-8E21BCE16101}"/>
+    <hyperlink ref="X10" r:id="rId31" xr:uid="{465D83FD-48FF-48EE-A4AA-EE7AF90F5BBD}"/>
+    <hyperlink ref="X11" r:id="rId32" xr:uid="{A8D2FF8B-A2A9-4B6F-B217-2E14C6EE9235}"/>
+    <hyperlink ref="M11" r:id="rId33" xr:uid="{175F9C8E-DB2C-48B2-B5D8-B249A4302B95}"/>
+    <hyperlink ref="X12" r:id="rId34" xr:uid="{E8D52455-2D02-474B-887B-F66CB5AB7BF3}"/>
+    <hyperlink ref="M12" r:id="rId35" xr:uid="{E9C6333C-597D-41EE-B1FC-1EE6178B208F}"/>
+    <hyperlink ref="X13" r:id="rId36" xr:uid="{8F2202D7-9DB8-441F-A802-398ADF2EFB9B}"/>
+    <hyperlink ref="M13" r:id="rId37" xr:uid="{5D30A358-A0BD-4F64-98E8-9F16E791B106}"/>
+    <hyperlink ref="X14" r:id="rId38" xr:uid="{104DBC51-97D1-4A7F-9676-DA2144C8BCF2}"/>
+    <hyperlink ref="M14" r:id="rId39" xr:uid="{D24A006E-62D8-4CFC-ADF2-379D45B10FF0}"/>
+    <hyperlink ref="X15" r:id="rId40" xr:uid="{D310A4E7-C9AA-43B0-8463-E957DE6367C0}"/>
+    <hyperlink ref="M15" r:id="rId41" xr:uid="{663D5588-CAD1-437B-8677-1C84B795019D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9008,8 +9118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BB1AD0-E1E7-4AA3-8FBD-385271ECBB27}">
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9650,7 +9760,7 @@
         <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C11" t="s">
         <v>346</v>
@@ -9683,7 +9793,7 @@
         <v>335</v>
       </c>
       <c r="M11" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="N11">
         <v>9876543210</v>

</xml_diff>

<commit_message>
Updated consignment ID for production.
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HardDiskCopied\E\InelliJ\SeleniumTestJavaArtifact2july\SeleniumTestJavaArtifact\DataFiles\excel\Login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D674765A-CB21-4591-8CF9-38BFA9ED5F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829C108B-2530-4D90-918E-84EDA0C1C9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="883" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="883" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EditConsignmentUAT" sheetId="10" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4346" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4391" uniqueCount="569">
   <si>
     <t>RunToTest</t>
   </si>
@@ -1729,6 +1729,15 @@
   </si>
   <si>
     <t>PROD00031010</t>
+  </si>
+  <si>
+    <t>PROD00021010</t>
+  </si>
+  <si>
+    <t>PROD00011007</t>
+  </si>
+  <si>
+    <t>PROD00031011</t>
   </si>
 </sst>
 </file>
@@ -9409,10 +9418,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE03A24-5145-4BFC-B798-CD5C2D481D00}">
   <dimension ref="A1:Z101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10169,7 +10178,7 @@
     </row>
     <row r="16" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>563</v>
@@ -10241,6 +10250,83 @@
         <v>30</v>
       </c>
       <c r="Z16" s="1">
+        <v>5.0255000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="H17" s="1">
+        <v>400</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="K17" s="1">
+        <v>3</v>
+      </c>
+      <c r="L17" s="1">
+        <v>3</v>
+      </c>
+      <c r="N17" s="1">
+        <v>40</v>
+      </c>
+      <c r="O17" s="1">
+        <v>45</v>
+      </c>
+      <c r="P17" s="1">
+        <v>52</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="S17" s="1">
+        <v>30</v>
+      </c>
+      <c r="T17" s="1">
+        <v>50</v>
+      </c>
+      <c r="U17" s="1">
+        <v>60</v>
+      </c>
+      <c r="V17" s="1">
+        <v>8.0779999999999994</v>
+      </c>
+      <c r="W17" s="1">
+        <v>60</v>
+      </c>
+      <c r="X17" s="1">
+        <v>50</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>30</v>
+      </c>
+      <c r="Z17" s="1">
         <v>5.0255000000000001</v>
       </c>
     </row>
@@ -10307,8 +10393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1FC442-2A76-4913-8893-A0FD6FAA9326}">
   <dimension ref="A1:X73"/>
   <sheetViews>
-    <sheetView topLeftCell="M11" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView topLeftCell="P11" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11365,7 +11451,7 @@
     </row>
     <row r="15" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>564</v>
@@ -11437,8 +11523,76 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="M16" s="2"/>
+    <row r="16" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
+        <v>567</v>
+      </c>
+      <c r="C16" t="s">
+        <v>346</v>
+      </c>
+      <c r="D16" t="s">
+        <v>341</v>
+      </c>
+      <c r="E16" t="s">
+        <v>342</v>
+      </c>
+      <c r="F16" t="s">
+        <v>332</v>
+      </c>
+      <c r="G16" t="s">
+        <v>107</v>
+      </c>
+      <c r="H16" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16" t="s">
+        <v>141</v>
+      </c>
+      <c r="J16" t="s">
+        <v>111</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L16" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="N16" t="s">
+        <v>359</v>
+      </c>
+      <c r="O16" t="s">
+        <v>343</v>
+      </c>
+      <c r="P16" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q16">
+        <v>123</v>
+      </c>
+      <c r="R16">
+        <v>987545555555555</v>
+      </c>
+      <c r="S16" t="s">
+        <v>124</v>
+      </c>
+      <c r="T16">
+        <v>1.11188888888888E+18</v>
+      </c>
+      <c r="U16" t="s">
+        <v>128</v>
+      </c>
+      <c r="V16" t="s">
+        <v>129</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
       <c r="X16" s="3" t="s">
         <v>116</v>
       </c>
@@ -11544,45 +11698,46 @@
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" xr:uid="{358998FA-15FF-431B-99C1-DF0C84EFB86F}"/>
     <hyperlink ref="X2" r:id="rId2" xr:uid="{AE14EEEB-3B83-40AE-9BDF-EA985C28F832}"/>
-    <hyperlink ref="X16" r:id="rId3" xr:uid="{19361FA6-9504-453F-92E7-DF6E9F4FA63D}"/>
-    <hyperlink ref="X17" r:id="rId4" xr:uid="{F402E61A-6BC9-41B2-87DF-C3A27E532E13}"/>
-    <hyperlink ref="X18" r:id="rId5" xr:uid="{43A3EAE1-5CC3-4836-A288-2BF5FC280717}"/>
-    <hyperlink ref="X19" r:id="rId6" xr:uid="{6F5EC072-9F18-4EC5-8DB2-2DF2CBF01CB0}"/>
-    <hyperlink ref="X20" r:id="rId7" xr:uid="{4CA5FEE5-0C07-4808-9248-B660743F3774}"/>
-    <hyperlink ref="X21" r:id="rId8" xr:uid="{ED490A4D-F92A-47BE-9867-4314A59BC6B7}"/>
-    <hyperlink ref="X22" r:id="rId9" xr:uid="{46880446-6A4E-403B-ADFA-CE8197023B30}"/>
-    <hyperlink ref="X23" r:id="rId10" xr:uid="{9524D2D4-0229-4303-A39E-B5869A5AB6F9}"/>
-    <hyperlink ref="X24" r:id="rId11" xr:uid="{918DE3BD-31B5-4450-94FD-FF0C378CE62A}"/>
-    <hyperlink ref="X25" r:id="rId12" xr:uid="{6DCC4064-F791-487D-8795-51EDAB204E8F}"/>
-    <hyperlink ref="X26" r:id="rId13" xr:uid="{CDB54460-A79F-4C90-B70B-EEBEE40D5E15}"/>
-    <hyperlink ref="X27" r:id="rId14" xr:uid="{020E49A6-F847-4012-A984-5906C66B24C2}"/>
-    <hyperlink ref="X28" r:id="rId15" xr:uid="{116CD7FA-45D6-45D0-9F78-90290FDE7EC3}"/>
-    <hyperlink ref="M3" r:id="rId16" xr:uid="{B6C5C0C4-A5CD-4989-9129-C8A7A85B04B8}"/>
-    <hyperlink ref="X3" r:id="rId17" xr:uid="{2F3B3A48-891E-47E7-8670-CEDB6572CA2B}"/>
-    <hyperlink ref="M4" r:id="rId18" xr:uid="{6A74C82A-96E6-471E-8814-621213BF313E}"/>
-    <hyperlink ref="X4" r:id="rId19" xr:uid="{FD29A6B0-0DCE-4017-BE5D-844FE8F434EA}"/>
-    <hyperlink ref="M5" r:id="rId20" xr:uid="{06767FBB-30D3-4571-B179-8F6EB3FEC4B4}"/>
-    <hyperlink ref="X5" r:id="rId21" xr:uid="{8840BE2F-FC00-482D-8632-9DB48E041BCA}"/>
-    <hyperlink ref="M6" r:id="rId22" xr:uid="{0A59FE27-88F7-4F24-A496-311F958815C8}"/>
-    <hyperlink ref="X6" r:id="rId23" xr:uid="{8DC3250D-4424-4A6C-B68D-FEC080B637FA}"/>
-    <hyperlink ref="M7" r:id="rId24" xr:uid="{4DC610F6-9A84-4368-BDF1-FF9BB2560852}"/>
-    <hyperlink ref="X7" r:id="rId25" xr:uid="{0FC8FA66-5837-4A59-BD4F-2E68649B972A}"/>
-    <hyperlink ref="M8" r:id="rId26" xr:uid="{88F825E6-41C8-4F6A-96AE-F0685382C2FB}"/>
-    <hyperlink ref="X8" r:id="rId27" xr:uid="{BF022674-73DC-417D-AA01-42951A83A5A9}"/>
-    <hyperlink ref="M9" r:id="rId28" xr:uid="{FA4C93BE-D55C-4CEF-901E-0EE7890E7319}"/>
-    <hyperlink ref="X9" r:id="rId29" xr:uid="{FE2E5242-2733-429A-B446-49922A127C38}"/>
-    <hyperlink ref="M10" r:id="rId30" xr:uid="{38AAA3EB-9E30-46B7-9C48-8E21BCE16101}"/>
-    <hyperlink ref="X10" r:id="rId31" xr:uid="{465D83FD-48FF-48EE-A4AA-EE7AF90F5BBD}"/>
-    <hyperlink ref="X11" r:id="rId32" xr:uid="{A8D2FF8B-A2A9-4B6F-B217-2E14C6EE9235}"/>
-    <hyperlink ref="M11" r:id="rId33" xr:uid="{175F9C8E-DB2C-48B2-B5D8-B249A4302B95}"/>
-    <hyperlink ref="X12" r:id="rId34" xr:uid="{E8D52455-2D02-474B-887B-F66CB5AB7BF3}"/>
-    <hyperlink ref="M12" r:id="rId35" xr:uid="{E9C6333C-597D-41EE-B1FC-1EE6178B208F}"/>
-    <hyperlink ref="X13" r:id="rId36" xr:uid="{8F2202D7-9DB8-441F-A802-398ADF2EFB9B}"/>
-    <hyperlink ref="M13" r:id="rId37" xr:uid="{5D30A358-A0BD-4F64-98E8-9F16E791B106}"/>
-    <hyperlink ref="X14" r:id="rId38" xr:uid="{104DBC51-97D1-4A7F-9676-DA2144C8BCF2}"/>
-    <hyperlink ref="M14" r:id="rId39" xr:uid="{D24A006E-62D8-4CFC-ADF2-379D45B10FF0}"/>
-    <hyperlink ref="X15" r:id="rId40" xr:uid="{EEBAAFBA-790C-4DDF-B14F-973B95084BB4}"/>
-    <hyperlink ref="M15" r:id="rId41" xr:uid="{3F639266-ADC2-4A0F-BD83-A1AB3881E65F}"/>
+    <hyperlink ref="X17" r:id="rId3" xr:uid="{F402E61A-6BC9-41B2-87DF-C3A27E532E13}"/>
+    <hyperlink ref="X18" r:id="rId4" xr:uid="{43A3EAE1-5CC3-4836-A288-2BF5FC280717}"/>
+    <hyperlink ref="X19" r:id="rId5" xr:uid="{6F5EC072-9F18-4EC5-8DB2-2DF2CBF01CB0}"/>
+    <hyperlink ref="X20" r:id="rId6" xr:uid="{4CA5FEE5-0C07-4808-9248-B660743F3774}"/>
+    <hyperlink ref="X21" r:id="rId7" xr:uid="{ED490A4D-F92A-47BE-9867-4314A59BC6B7}"/>
+    <hyperlink ref="X22" r:id="rId8" xr:uid="{46880446-6A4E-403B-ADFA-CE8197023B30}"/>
+    <hyperlink ref="X23" r:id="rId9" xr:uid="{9524D2D4-0229-4303-A39E-B5869A5AB6F9}"/>
+    <hyperlink ref="X24" r:id="rId10" xr:uid="{918DE3BD-31B5-4450-94FD-FF0C378CE62A}"/>
+    <hyperlink ref="X25" r:id="rId11" xr:uid="{6DCC4064-F791-487D-8795-51EDAB204E8F}"/>
+    <hyperlink ref="X26" r:id="rId12" xr:uid="{CDB54460-A79F-4C90-B70B-EEBEE40D5E15}"/>
+    <hyperlink ref="X27" r:id="rId13" xr:uid="{020E49A6-F847-4012-A984-5906C66B24C2}"/>
+    <hyperlink ref="X28" r:id="rId14" xr:uid="{116CD7FA-45D6-45D0-9F78-90290FDE7EC3}"/>
+    <hyperlink ref="M3" r:id="rId15" xr:uid="{B6C5C0C4-A5CD-4989-9129-C8A7A85B04B8}"/>
+    <hyperlink ref="X3" r:id="rId16" xr:uid="{2F3B3A48-891E-47E7-8670-CEDB6572CA2B}"/>
+    <hyperlink ref="M4" r:id="rId17" xr:uid="{6A74C82A-96E6-471E-8814-621213BF313E}"/>
+    <hyperlink ref="X4" r:id="rId18" xr:uid="{FD29A6B0-0DCE-4017-BE5D-844FE8F434EA}"/>
+    <hyperlink ref="M5" r:id="rId19" xr:uid="{06767FBB-30D3-4571-B179-8F6EB3FEC4B4}"/>
+    <hyperlink ref="X5" r:id="rId20" xr:uid="{8840BE2F-FC00-482D-8632-9DB48E041BCA}"/>
+    <hyperlink ref="M6" r:id="rId21" xr:uid="{0A59FE27-88F7-4F24-A496-311F958815C8}"/>
+    <hyperlink ref="X6" r:id="rId22" xr:uid="{8DC3250D-4424-4A6C-B68D-FEC080B637FA}"/>
+    <hyperlink ref="M7" r:id="rId23" xr:uid="{4DC610F6-9A84-4368-BDF1-FF9BB2560852}"/>
+    <hyperlink ref="X7" r:id="rId24" xr:uid="{0FC8FA66-5837-4A59-BD4F-2E68649B972A}"/>
+    <hyperlink ref="M8" r:id="rId25" xr:uid="{88F825E6-41C8-4F6A-96AE-F0685382C2FB}"/>
+    <hyperlink ref="X8" r:id="rId26" xr:uid="{BF022674-73DC-417D-AA01-42951A83A5A9}"/>
+    <hyperlink ref="M9" r:id="rId27" xr:uid="{FA4C93BE-D55C-4CEF-901E-0EE7890E7319}"/>
+    <hyperlink ref="X9" r:id="rId28" xr:uid="{FE2E5242-2733-429A-B446-49922A127C38}"/>
+    <hyperlink ref="M10" r:id="rId29" xr:uid="{38AAA3EB-9E30-46B7-9C48-8E21BCE16101}"/>
+    <hyperlink ref="X10" r:id="rId30" xr:uid="{465D83FD-48FF-48EE-A4AA-EE7AF90F5BBD}"/>
+    <hyperlink ref="X11" r:id="rId31" xr:uid="{A8D2FF8B-A2A9-4B6F-B217-2E14C6EE9235}"/>
+    <hyperlink ref="M11" r:id="rId32" xr:uid="{175F9C8E-DB2C-48B2-B5D8-B249A4302B95}"/>
+    <hyperlink ref="X12" r:id="rId33" xr:uid="{E8D52455-2D02-474B-887B-F66CB5AB7BF3}"/>
+    <hyperlink ref="M12" r:id="rId34" xr:uid="{E9C6333C-597D-41EE-B1FC-1EE6178B208F}"/>
+    <hyperlink ref="X13" r:id="rId35" xr:uid="{8F2202D7-9DB8-441F-A802-398ADF2EFB9B}"/>
+    <hyperlink ref="M13" r:id="rId36" xr:uid="{5D30A358-A0BD-4F64-98E8-9F16E791B106}"/>
+    <hyperlink ref="X14" r:id="rId37" xr:uid="{104DBC51-97D1-4A7F-9676-DA2144C8BCF2}"/>
+    <hyperlink ref="M14" r:id="rId38" xr:uid="{D24A006E-62D8-4CFC-ADF2-379D45B10FF0}"/>
+    <hyperlink ref="X15" r:id="rId39" xr:uid="{EEBAAFBA-790C-4DDF-B14F-973B95084BB4}"/>
+    <hyperlink ref="M15" r:id="rId40" xr:uid="{3F639266-ADC2-4A0F-BD83-A1AB3881E65F}"/>
+    <hyperlink ref="X16" r:id="rId41" xr:uid="{8D52F66F-F853-4C97-8FCB-310C0712816A}"/>
+    <hyperlink ref="M16" r:id="rId42" xr:uid="{4A84D3DC-9E57-4918-A6C6-54B0B826E194}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11592,10 +11747,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BB1AD0-E1E7-4AA3-8FBD-385271ECBB27}">
   <dimension ref="A1:AH73"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O1" sqref="O1"/>
-      <selection pane="bottomLeft" activeCell="W15" sqref="W15"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12688,7 +12843,7 @@
     </row>
     <row r="15" spans="1:34" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>565</v>
@@ -12790,10 +12945,109 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="O16" s="2"/>
+    <row r="16" spans="1:34" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
+        <v>568</v>
+      </c>
+      <c r="C16" t="s">
+        <v>346</v>
+      </c>
+      <c r="D16" t="s">
+        <v>347</v>
+      </c>
+      <c r="E16" t="s">
+        <v>348</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="G16" t="s">
+        <v>138</v>
+      </c>
+      <c r="H16" t="s">
+        <v>141</v>
+      </c>
+      <c r="I16" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="L16" t="s">
+        <v>335</v>
+      </c>
+      <c r="M16" t="s">
+        <v>480</v>
+      </c>
+      <c r="N16">
+        <v>9876543210</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="P16">
+        <v>107</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>156</v>
+      </c>
+      <c r="R16" t="s">
+        <v>129</v>
+      </c>
+      <c r="S16" t="s">
+        <v>148</v>
+      </c>
+      <c r="T16">
+        <v>4</v>
+      </c>
+      <c r="U16">
+        <v>25</v>
+      </c>
+      <c r="V16">
+        <v>30</v>
+      </c>
+      <c r="W16">
+        <v>35</v>
+      </c>
+      <c r="X16">
+        <v>1.52</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>497</v>
+      </c>
+      <c r="Z16">
+        <v>6</v>
+      </c>
+      <c r="AA16">
+        <v>8</v>
+      </c>
+      <c r="AB16">
+        <v>7</v>
+      </c>
+      <c r="AC16">
+        <v>1.256</v>
+      </c>
+      <c r="AD16">
+        <v>5</v>
+      </c>
+      <c r="AE16">
+        <v>8</v>
+      </c>
+      <c r="AF16">
+        <v>12</v>
+      </c>
+      <c r="AG16">
+        <v>1.78</v>
+      </c>
+      <c r="AH16">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="10:15" x14ac:dyDescent="0.25">
       <c r="J17" s="2"/>
@@ -13326,6 +13580,8 @@
     <hyperlink ref="O14" r:id="rId26" xr:uid="{C9854A30-1431-4A71-91D0-7578FC50B844}"/>
     <hyperlink ref="J15" r:id="rId27" xr:uid="{04633D87-9E4C-4B18-851E-1CAF73816960}"/>
     <hyperlink ref="O15" r:id="rId28" xr:uid="{6EEABB60-7AB3-42D9-9ADF-9E10D159DB0B}"/>
+    <hyperlink ref="J16" r:id="rId29" xr:uid="{63E0615C-2480-4542-AA8D-B37B335F03DE}"/>
+    <hyperlink ref="O16" r:id="rId30" xr:uid="{EFA3265C-6B58-4700-B674-7A79F60486D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
1st March- Added headless code on chromeBrowser
</commit_message>
<xml_diff>
--- a/DataFiles/excel/Login/ConsignmentDetails.xlsx
+++ b/DataFiles/excel/Login/ConsignmentDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nasreen\HardDiskCopied\E\InelliJ\SeleniumTestJavaArtifact2july\SeleniumTestJavaArtifact\DataFiles\excel\Login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33903696-E1D7-4209-8E93-E5D8B4463E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C8CF1A-F9F7-4127-92BC-FAFFE5BA31CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="836" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="836" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EditConsignmentUAT" sheetId="10" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4423" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4718" uniqueCount="609">
   <si>
     <t>RunToTest</t>
   </si>
@@ -1784,6 +1784,84 @@
   </si>
   <si>
     <t>UAT00311003</t>
+  </si>
+  <si>
+    <t>UAT07100153</t>
+  </si>
+  <si>
+    <t>UAT42092279</t>
+  </si>
+  <si>
+    <t>UAT08000139</t>
+  </si>
+  <si>
+    <t>UAT08000140</t>
+  </si>
+  <si>
+    <t>UAT07100154</t>
+  </si>
+  <si>
+    <t>UAT07100155</t>
+  </si>
+  <si>
+    <t>UAT00311004</t>
+  </si>
+  <si>
+    <t>UAT42092300</t>
+  </si>
+  <si>
+    <t>UAT00211005</t>
+  </si>
+  <si>
+    <t>UAT00211006</t>
+  </si>
+  <si>
+    <t>UAT00211007</t>
+  </si>
+  <si>
+    <t>UAT00211008</t>
+  </si>
+  <si>
+    <t>UAT00211009</t>
+  </si>
+  <si>
+    <t>UAT00211010</t>
+  </si>
+  <si>
+    <t>UAT00311010</t>
+  </si>
+  <si>
+    <t>UAT00211011</t>
+  </si>
+  <si>
+    <t>UAT00311011</t>
+  </si>
+  <si>
+    <t>UAT42092301</t>
+  </si>
+  <si>
+    <t>UAT07100156</t>
+  </si>
+  <si>
+    <t>UAT00211012</t>
+  </si>
+  <si>
+    <t>UAT00311012</t>
+  </si>
+  <si>
+    <t>UAT42092302</t>
+  </si>
+  <si>
+    <t>UAT08000141</t>
+  </si>
+  <si>
+    <t>UAT07100157</t>
+  </si>
+  <si>
+    <t>UAT00211013</t>
+  </si>
+  <si>
+    <t>UAT00311013</t>
   </si>
 </sst>
 </file>
@@ -2516,7 +2594,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2620,11 +2698,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB156"/>
+  <dimension ref="A1:AB160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A155" sqref="A155"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B160" sqref="B160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9640,7 +9718,7 @@
     </row>
     <row r="156" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>555</v>
@@ -9721,6 +9799,350 @@
         <v>60</v>
       </c>
       <c r="AB156" s="1">
+        <v>8.0779999999999994</v>
+      </c>
+    </row>
+    <row r="157" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H157" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I157" s="1">
+        <v>456</v>
+      </c>
+      <c r="J157" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="K157" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="L157" s="1">
+        <v>1</v>
+      </c>
+      <c r="M157" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N157" s="1">
+        <v>60</v>
+      </c>
+      <c r="O157" s="1">
+        <v>50</v>
+      </c>
+      <c r="P157" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q157" s="1">
+        <v>5.0255000000000001</v>
+      </c>
+      <c r="R157" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="S157" s="1">
+        <v>1</v>
+      </c>
+      <c r="T157" s="1">
+        <v>35</v>
+      </c>
+      <c r="U157" s="1">
+        <v>40</v>
+      </c>
+      <c r="V157" s="1">
+        <v>52</v>
+      </c>
+      <c r="W157" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="X157" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="Y157" s="1">
+        <v>30</v>
+      </c>
+      <c r="Z157" s="1">
+        <v>50</v>
+      </c>
+      <c r="AA157" s="1">
+        <v>60</v>
+      </c>
+      <c r="AB157" s="1">
+        <v>8.0779999999999994</v>
+      </c>
+    </row>
+    <row r="158" spans="1:28" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H158" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I158" s="1">
+        <v>456</v>
+      </c>
+      <c r="J158" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="K158" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="L158" s="1">
+        <v>1</v>
+      </c>
+      <c r="M158" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N158" s="1">
+        <v>60</v>
+      </c>
+      <c r="O158" s="1">
+        <v>50</v>
+      </c>
+      <c r="P158" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q158" s="1">
+        <v>5.0255000000000001</v>
+      </c>
+      <c r="R158" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="S158" s="1">
+        <v>1</v>
+      </c>
+      <c r="T158" s="1">
+        <v>35</v>
+      </c>
+      <c r="U158" s="1">
+        <v>40</v>
+      </c>
+      <c r="V158" s="1">
+        <v>52</v>
+      </c>
+      <c r="W158" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="X158" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="Y158" s="1">
+        <v>30</v>
+      </c>
+      <c r="Z158" s="1">
+        <v>50</v>
+      </c>
+      <c r="AA158" s="1">
+        <v>60</v>
+      </c>
+      <c r="AB158" s="1">
+        <v>8.0779999999999994</v>
+      </c>
+    </row>
+    <row r="159" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G159" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H159" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I159" s="1">
+        <v>456</v>
+      </c>
+      <c r="J159" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="K159" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="L159" s="1">
+        <v>1</v>
+      </c>
+      <c r="M159" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N159" s="1">
+        <v>60</v>
+      </c>
+      <c r="O159" s="1">
+        <v>50</v>
+      </c>
+      <c r="P159" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q159" s="1">
+        <v>5.0255000000000001</v>
+      </c>
+      <c r="R159" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="S159" s="1">
+        <v>1</v>
+      </c>
+      <c r="T159" s="1">
+        <v>35</v>
+      </c>
+      <c r="U159" s="1">
+        <v>40</v>
+      </c>
+      <c r="V159" s="1">
+        <v>52</v>
+      </c>
+      <c r="W159" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="X159" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="Y159" s="1">
+        <v>30</v>
+      </c>
+      <c r="Z159" s="1">
+        <v>50</v>
+      </c>
+      <c r="AA159" s="1">
+        <v>60</v>
+      </c>
+      <c r="AB159" s="1">
+        <v>8.0779999999999994</v>
+      </c>
+    </row>
+    <row r="160" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G160" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H160" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I160" s="1">
+        <v>456</v>
+      </c>
+      <c r="J160" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="K160" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="L160" s="1">
+        <v>1</v>
+      </c>
+      <c r="M160" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N160" s="1">
+        <v>60</v>
+      </c>
+      <c r="O160" s="1">
+        <v>50</v>
+      </c>
+      <c r="P160" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q160" s="1">
+        <v>5.0255000000000001</v>
+      </c>
+      <c r="R160" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="S160" s="1">
+        <v>1</v>
+      </c>
+      <c r="T160" s="1">
+        <v>35</v>
+      </c>
+      <c r="U160" s="1">
+        <v>40</v>
+      </c>
+      <c r="V160" s="1">
+        <v>52</v>
+      </c>
+      <c r="W160" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="X160" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="Y160" s="1">
+        <v>30</v>
+      </c>
+      <c r="Z160" s="1">
+        <v>50</v>
+      </c>
+      <c r="AA160" s="1">
+        <v>60</v>
+      </c>
+      <c r="AB160" s="1">
         <v>8.0779999999999994</v>
       </c>
     </row>
@@ -13413,9 +13835,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X73"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16470,7 +16892,7 @@
     </row>
     <row r="42" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
         <v>542</v>
@@ -16542,96 +16964,300 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>28</v>
       </c>
+      <c r="B43" t="s">
+        <v>585</v>
+      </c>
       <c r="C43" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D43" t="s">
+        <v>102</v>
+      </c>
+      <c r="E43" t="s">
+        <v>104</v>
+      </c>
+      <c r="F43" t="s">
+        <v>126</v>
+      </c>
+      <c r="G43" t="s">
+        <v>107</v>
+      </c>
+      <c r="H43" t="s">
+        <v>560</v>
+      </c>
+      <c r="I43" t="s">
+        <v>561</v>
+      </c>
+      <c r="J43" t="s">
+        <v>111</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L43" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N43" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O43" t="s">
+        <v>119</v>
+      </c>
+      <c r="P43" t="s">
+        <v>559</v>
       </c>
       <c r="Q43">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R43">
+        <v>987545555555555</v>
+      </c>
+      <c r="S43" t="s">
+        <v>124</v>
+      </c>
+      <c r="T43">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U43" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V43" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X43" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>28</v>
       </c>
+      <c r="B44" t="s">
+        <v>586</v>
+      </c>
       <c r="C44" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D44" t="s">
+        <v>102</v>
+      </c>
+      <c r="E44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F44" t="s">
+        <v>126</v>
+      </c>
+      <c r="G44" t="s">
+        <v>107</v>
+      </c>
+      <c r="H44" t="s">
+        <v>560</v>
+      </c>
+      <c r="I44" t="s">
+        <v>561</v>
+      </c>
+      <c r="J44" t="s">
+        <v>111</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L44" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N44" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O44" t="s">
+        <v>119</v>
+      </c>
+      <c r="P44" t="s">
+        <v>559</v>
       </c>
       <c r="Q44">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R44">
+        <v>987545555555555</v>
+      </c>
+      <c r="S44" t="s">
+        <v>124</v>
+      </c>
+      <c r="T44">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U44" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V44" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X44" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>28</v>
       </c>
+      <c r="B45" t="s">
+        <v>586</v>
+      </c>
       <c r="C45" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D45" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" t="s">
+        <v>104</v>
+      </c>
+      <c r="F45" t="s">
+        <v>126</v>
+      </c>
+      <c r="G45" t="s">
+        <v>107</v>
+      </c>
+      <c r="H45" t="s">
+        <v>560</v>
+      </c>
+      <c r="I45" t="s">
+        <v>561</v>
+      </c>
+      <c r="J45" t="s">
+        <v>111</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L45" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N45" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O45" t="s">
+        <v>119</v>
+      </c>
+      <c r="P45" t="s">
+        <v>559</v>
       </c>
       <c r="Q45">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R45">
+        <v>987545555555555</v>
+      </c>
+      <c r="S45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T45">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U45" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V45" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="X45" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
+        <v>605</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>125</v>
+      </c>
+      <c r="D46" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46" t="s">
+        <v>104</v>
+      </c>
+      <c r="F46" t="s">
+        <v>126</v>
+      </c>
+      <c r="G46" t="s">
+        <v>107</v>
+      </c>
+      <c r="H46" t="s">
+        <v>560</v>
+      </c>
+      <c r="I46" t="s">
+        <v>561</v>
+      </c>
+      <c r="J46" t="s">
+        <v>111</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L46" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="N46" t="s">
-        <v>7</v>
+        <v>96</v>
+      </c>
+      <c r="O46" t="s">
+        <v>119</v>
+      </c>
+      <c r="P46" t="s">
+        <v>559</v>
       </c>
       <c r="Q46">
-        <v>456</v>
+        <v>123</v>
+      </c>
+      <c r="R46">
+        <v>987545555555555</v>
+      </c>
+      <c r="S46" t="s">
+        <v>124</v>
+      </c>
+      <c r="T46">
+        <v>1.11188888888888E+18</v>
       </c>
       <c r="U46" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="V46" t="s">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="W46">
         <v>1</v>
+      </c>
+      <c r="X46" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -17375,9 +18001,17 @@
     <hyperlink ref="X41" r:id="rId80" xr:uid="{B54F2C96-A187-4B3D-BEC5-5A0E0F62E2B9}"/>
     <hyperlink ref="M42" r:id="rId81" xr:uid="{1A7F4856-F6A5-4EE0-B2BB-076779DA75E3}"/>
     <hyperlink ref="X42" r:id="rId82" xr:uid="{552A02B3-D49B-44BD-99DC-743CAEBCAFC0}"/>
+    <hyperlink ref="M43" r:id="rId83" xr:uid="{2BEE92F8-DE31-48A9-8813-98E7FE7DE461}"/>
+    <hyperlink ref="X43" r:id="rId84" xr:uid="{B092815E-F7D9-4F0A-A205-23973769F2D4}"/>
+    <hyperlink ref="M44" r:id="rId85" xr:uid="{F18420CC-7B4B-4AB1-B662-A1570A846DB8}"/>
+    <hyperlink ref="X44" r:id="rId86" xr:uid="{44DEDF77-7BDA-457D-B05C-2F662405AA86}"/>
+    <hyperlink ref="M45" r:id="rId87" xr:uid="{14E59667-257B-4A45-8F5B-25EF91D92398}"/>
+    <hyperlink ref="X45" r:id="rId88" xr:uid="{0EDC542C-B3ED-43F4-B652-FBF1C7088B2B}"/>
+    <hyperlink ref="M46" r:id="rId89" xr:uid="{A88B78A8-C71D-4D49-8AFE-B6009577BA10}"/>
+    <hyperlink ref="X46" r:id="rId90" xr:uid="{1DFFD102-6D13-428F-804F-686AEACE2B40}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId83"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId91"/>
 </worksheet>
 </file>
 
@@ -17386,9 +18020,9 @@
   <dimension ref="A1:AH73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
+      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21438,7 +22072,7 @@
     </row>
     <row r="54" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B54" t="s">
         <v>562</v>
@@ -21540,74 +22174,524 @@
         <v>1.256</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>28</v>
       </c>
+      <c r="B55" t="s">
+        <v>583</v>
+      </c>
       <c r="C55" t="s">
-        <v>94</v>
-      </c>
-      <c r="N55" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D55" t="s">
+        <v>102</v>
+      </c>
+      <c r="E55" t="s">
+        <v>138</v>
+      </c>
+      <c r="F55" t="s">
+        <v>565</v>
+      </c>
+      <c r="G55" t="s">
+        <v>138</v>
+      </c>
+      <c r="H55" t="s">
+        <v>141</v>
+      </c>
+      <c r="I55" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K55" t="s">
+        <v>563</v>
+      </c>
+      <c r="L55" t="s">
+        <v>564</v>
+      </c>
+      <c r="M55">
+        <v>9876543210</v>
+      </c>
+      <c r="N55" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O55">
+        <v>107</v>
+      </c>
+      <c r="P55" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>129</v>
+      </c>
+      <c r="R55" t="s">
+        <v>148</v>
       </c>
       <c r="S55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="T55">
+        <v>2</v>
+      </c>
+      <c r="U55">
+        <v>3</v>
+      </c>
+      <c r="V55">
+        <v>8</v>
+      </c>
+      <c r="W55">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="X55" t="s">
+        <v>489</v>
+      </c>
+      <c r="Y55">
+        <v>4</v>
+      </c>
+      <c r="Z55">
+        <v>25</v>
+      </c>
+      <c r="AA55">
+        <v>30</v>
+      </c>
+      <c r="AB55">
+        <v>35</v>
+      </c>
+      <c r="AC55">
+        <v>1.52</v>
+      </c>
+      <c r="AD55" t="s">
+        <v>497</v>
+      </c>
+      <c r="AE55">
+        <v>6</v>
+      </c>
+      <c r="AF55">
+        <v>8</v>
+      </c>
+      <c r="AG55">
+        <v>7</v>
+      </c>
+      <c r="AH55">
+        <v>1.256</v>
+      </c>
+    </row>
+    <row r="56" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>28</v>
       </c>
+      <c r="B56" t="s">
+        <v>587</v>
+      </c>
       <c r="C56" t="s">
-        <v>94</v>
-      </c>
-      <c r="N56" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D56" t="s">
+        <v>102</v>
+      </c>
+      <c r="E56" t="s">
+        <v>138</v>
+      </c>
+      <c r="F56" t="s">
+        <v>565</v>
+      </c>
+      <c r="G56" t="s">
+        <v>138</v>
+      </c>
+      <c r="H56" t="s">
+        <v>141</v>
+      </c>
+      <c r="I56" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K56" t="s">
+        <v>563</v>
+      </c>
+      <c r="L56" t="s">
+        <v>564</v>
+      </c>
+      <c r="M56">
+        <v>9876543210</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O56">
+        <v>107</v>
+      </c>
+      <c r="P56" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>129</v>
+      </c>
+      <c r="R56" t="s">
+        <v>148</v>
       </c>
       <c r="S56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="T56">
+        <v>2</v>
+      </c>
+      <c r="U56">
+        <v>3</v>
+      </c>
+      <c r="V56">
+        <v>8</v>
+      </c>
+      <c r="W56">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="X56" t="s">
+        <v>489</v>
+      </c>
+      <c r="Y56">
+        <v>4</v>
+      </c>
+      <c r="Z56">
+        <v>25</v>
+      </c>
+      <c r="AA56">
+        <v>30</v>
+      </c>
+      <c r="AB56">
+        <v>35</v>
+      </c>
+      <c r="AC56">
+        <v>1.52</v>
+      </c>
+      <c r="AD56" t="s">
+        <v>497</v>
+      </c>
+      <c r="AE56">
+        <v>6</v>
+      </c>
+      <c r="AF56">
+        <v>8</v>
+      </c>
+      <c r="AG56">
+        <v>7</v>
+      </c>
+      <c r="AH56">
+        <v>1.256</v>
+      </c>
+    </row>
+    <row r="57" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>28</v>
       </c>
+      <c r="B57" t="s">
+        <v>588</v>
+      </c>
       <c r="C57" t="s">
-        <v>94</v>
-      </c>
-      <c r="N57" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D57" t="s">
+        <v>102</v>
+      </c>
+      <c r="E57" t="s">
+        <v>138</v>
+      </c>
+      <c r="F57" t="s">
+        <v>565</v>
+      </c>
+      <c r="G57" t="s">
+        <v>138</v>
+      </c>
+      <c r="H57" t="s">
+        <v>141</v>
+      </c>
+      <c r="I57" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K57" t="s">
+        <v>563</v>
+      </c>
+      <c r="L57" t="s">
+        <v>564</v>
+      </c>
+      <c r="M57">
+        <v>9876543210</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O57">
+        <v>107</v>
+      </c>
+      <c r="P57" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>129</v>
+      </c>
+      <c r="R57" t="s">
+        <v>148</v>
       </c>
       <c r="S57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="T57">
+        <v>2</v>
+      </c>
+      <c r="U57">
+        <v>3</v>
+      </c>
+      <c r="V57">
+        <v>8</v>
+      </c>
+      <c r="W57">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="X57" t="s">
+        <v>489</v>
+      </c>
+      <c r="Y57">
+        <v>4</v>
+      </c>
+      <c r="Z57">
+        <v>25</v>
+      </c>
+      <c r="AA57">
+        <v>30</v>
+      </c>
+      <c r="AB57">
+        <v>35</v>
+      </c>
+      <c r="AC57">
+        <v>1.52</v>
+      </c>
+      <c r="AD57" t="s">
+        <v>497</v>
+      </c>
+      <c r="AE57">
+        <v>6</v>
+      </c>
+      <c r="AF57">
+        <v>8</v>
+      </c>
+      <c r="AG57">
+        <v>7</v>
+      </c>
+      <c r="AH57">
+        <v>1.256</v>
+      </c>
+    </row>
+    <row r="58" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>28</v>
       </c>
+      <c r="B58" t="s">
+        <v>601</v>
+      </c>
       <c r="C58" t="s">
-        <v>94</v>
-      </c>
-      <c r="N58" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D58" t="s">
+        <v>102</v>
+      </c>
+      <c r="E58" t="s">
+        <v>138</v>
+      </c>
+      <c r="F58" t="s">
+        <v>565</v>
+      </c>
+      <c r="G58" t="s">
+        <v>138</v>
+      </c>
+      <c r="H58" t="s">
+        <v>141</v>
+      </c>
+      <c r="I58" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K58" t="s">
+        <v>563</v>
+      </c>
+      <c r="L58" t="s">
+        <v>564</v>
+      </c>
+      <c r="M58">
+        <v>9876543210</v>
+      </c>
+      <c r="N58" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O58">
+        <v>107</v>
+      </c>
+      <c r="P58" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>129</v>
+      </c>
+      <c r="R58" t="s">
+        <v>148</v>
       </c>
       <c r="S58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="T58">
+        <v>2</v>
+      </c>
+      <c r="U58">
+        <v>3</v>
+      </c>
+      <c r="V58">
+        <v>8</v>
+      </c>
+      <c r="W58">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="X58" t="s">
+        <v>489</v>
+      </c>
+      <c r="Y58">
+        <v>4</v>
+      </c>
+      <c r="Z58">
+        <v>25</v>
+      </c>
+      <c r="AA58">
+        <v>30</v>
+      </c>
+      <c r="AB58">
+        <v>35</v>
+      </c>
+      <c r="AC58">
+        <v>1.52</v>
+      </c>
+      <c r="AD58" t="s">
+        <v>497</v>
+      </c>
+      <c r="AE58">
+        <v>6</v>
+      </c>
+      <c r="AF58">
+        <v>8</v>
+      </c>
+      <c r="AG58">
+        <v>7</v>
+      </c>
+      <c r="AH58">
+        <v>1.256</v>
+      </c>
+    </row>
+    <row r="59" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>28</v>
+        <v>91</v>
+      </c>
+      <c r="B59" t="s">
+        <v>606</v>
       </c>
       <c r="C59" t="s">
-        <v>94</v>
-      </c>
-      <c r="N59" s="1">
-        <v>456</v>
+        <v>125</v>
+      </c>
+      <c r="D59" t="s">
+        <v>102</v>
+      </c>
+      <c r="E59" t="s">
+        <v>138</v>
+      </c>
+      <c r="F59" t="s">
+        <v>565</v>
+      </c>
+      <c r="G59" t="s">
+        <v>138</v>
+      </c>
+      <c r="H59" t="s">
+        <v>141</v>
+      </c>
+      <c r="I59" s="1">
+        <v>9848655555</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K59" t="s">
+        <v>563</v>
+      </c>
+      <c r="L59" t="s">
+        <v>564</v>
+      </c>
+      <c r="M59">
+        <v>9876543210</v>
+      </c>
+      <c r="N59" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O59">
+        <v>107</v>
+      </c>
+      <c r="P59" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>129</v>
+      </c>
+      <c r="R59" t="s">
+        <v>148</v>
       </c>
       <c r="S59">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="T59">
+        <v>2</v>
+      </c>
+      <c r="U59">
+        <v>3</v>
+      </c>
+      <c r="V59">
+        <v>8</v>
+      </c>
+      <c r="W59">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="X59" t="s">
+        <v>489</v>
+      </c>
+      <c r="Y59">
+        <v>4</v>
+      </c>
+      <c r="Z59">
+        <v>25</v>
+      </c>
+      <c r="AA59">
+        <v>30</v>
+      </c>
+      <c r="AB59">
+        <v>35</v>
+      </c>
+      <c r="AC59">
+        <v>1.52</v>
+      </c>
+      <c r="AD59" t="s">
+        <v>497</v>
+      </c>
+      <c r="AE59">
+        <v>6</v>
+      </c>
+      <c r="AF59">
+        <v>8</v>
+      </c>
+      <c r="AG59">
+        <v>7</v>
+      </c>
+      <c r="AH59">
+        <v>1.256</v>
       </c>
     </row>
     <row r="60" spans="1:34" x14ac:dyDescent="0.3">
@@ -21914,18 +22998,28 @@
     <hyperlink ref="N53" r:id="rId104" xr:uid="{255CED8A-E5BC-4527-BF46-30A74545D586}"/>
     <hyperlink ref="J54" r:id="rId105" xr:uid="{662F4EA2-7CA0-47DA-A30F-D6083B43578D}"/>
     <hyperlink ref="N54" r:id="rId106" xr:uid="{F3147A81-02A2-427F-95DC-49580580B558}"/>
+    <hyperlink ref="J55" r:id="rId107" xr:uid="{D45CE002-3EAC-4D63-982F-D65B6629C8AB}"/>
+    <hyperlink ref="N55" r:id="rId108" xr:uid="{E0434404-5AC2-49E1-A114-DAE28E5E26D4}"/>
+    <hyperlink ref="J56" r:id="rId109" xr:uid="{FF8D0597-9645-449F-823C-9F9B29154E0B}"/>
+    <hyperlink ref="N56" r:id="rId110" xr:uid="{A38058FE-FC56-4661-BB0C-1C9F6385FA0A}"/>
+    <hyperlink ref="J57" r:id="rId111" xr:uid="{F25BBA15-027E-4285-8783-4A2061FFA880}"/>
+    <hyperlink ref="N57" r:id="rId112" xr:uid="{33953300-7632-4C41-8997-BDBD0E782D9D}"/>
+    <hyperlink ref="J58" r:id="rId113" xr:uid="{43FEE378-A61D-4D50-9FD6-9D48C614E96B}"/>
+    <hyperlink ref="N58" r:id="rId114" xr:uid="{8CCDF921-B77B-4122-995E-94A0A1FF951E}"/>
+    <hyperlink ref="J59" r:id="rId115" xr:uid="{03EF0337-BA47-4651-BF5E-FF10B9718507}"/>
+    <hyperlink ref="N59" r:id="rId116" xr:uid="{401EE075-CA01-4A77-9342-0F388E1FEA15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId107"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId117"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9603E3-1555-46FB-BCC7-D3A0DADC829D}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22059,7 +23153,7 @@
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>581</v>
@@ -22083,6 +23177,296 @@
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1324</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1324</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1324</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1324</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1324</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1324</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1324</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1324</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1324</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1324</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -22093,10 +23477,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B3B5C8-4477-4678-9556-D1FB6FFD9127}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22230,7 +23614,7 @@
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>582</v>
@@ -22254,6 +23638,180 @@
         <v>2</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G6" t="s">
+        <v>572</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G7" t="s">
+        <v>572</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G8" t="s">
+        <v>572</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G9" t="s">
+        <v>572</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G10" t="s">
+        <v>572</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G11" t="s">
+        <v>572</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>573</v>
       </c>
     </row>
@@ -22263,6 +23821,12 @@
     <hyperlink ref="I3" r:id="rId2" xr:uid="{6DE8ADA7-4056-41C2-BE37-99E81A501A29}"/>
     <hyperlink ref="I4" r:id="rId3" xr:uid="{7BF3755E-1F7F-4ED8-978E-FAD443657123}"/>
     <hyperlink ref="I5" r:id="rId4" xr:uid="{441CEC14-AA60-4E5D-B547-0FB4BEFA2330}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{2C4D8BCC-4640-413A-8FF7-7AB220499432}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{37948B21-DF3C-4CC2-9085-CC2619654ABC}"/>
+    <hyperlink ref="I8" r:id="rId7" xr:uid="{4C3D81F5-F7B2-4429-B845-6197AD65790E}"/>
+    <hyperlink ref="I9" r:id="rId8" xr:uid="{D49BDF56-CE40-4F57-91B8-97A21B63D5C5}"/>
+    <hyperlink ref="I10" r:id="rId9" xr:uid="{9D48AA53-9D34-4665-8C22-2F207E85409C}"/>
+    <hyperlink ref="I11" r:id="rId10" xr:uid="{7719280A-E8E2-4960-AC66-9044E3BD3E94}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>